<commit_message>
Updating annual report disease lookup
</commit_message>
<xml_diff>
--- a/inst/diseases/disease_lookup.xlsx
+++ b/inst/diseases/disease_lookup.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmamendelsohn/r_projects/wahis/inst/diseases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDCCD7D-57B4-9E49-B363-0954DFDEA31D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3D5A07-2058-5545-BA5C-701221C36923}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11880" yWindow="-21140" windowWidth="14460" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="disease_lookup" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">disease_lookup!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">disease_lookup!$A$1:$F$349</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="599">
   <si>
     <t>disease</t>
   </si>
@@ -1264,15 +1264,9 @@
     <t>fowlpox</t>
   </si>
   <si>
-    <t>aujeszky¬¨√≠s disease</t>
-  </si>
-  <si>
     <t>ma45</t>
   </si>
   <si>
-    <t>aujeszky's disease</t>
-  </si>
-  <si>
     <t>porcine reproductive and respiratory syndrome</t>
   </si>
   <si>
@@ -1781,6 +1775,51 @@
   </si>
   <si>
     <t>ma182</t>
+  </si>
+  <si>
+    <t>aujeszkys disease</t>
+  </si>
+  <si>
+    <t>ag116</t>
+  </si>
+  <si>
+    <t>taylorella equigenitalis</t>
+  </si>
+  <si>
+    <t>ma163</t>
+  </si>
+  <si>
+    <t>contagious ecthyma</t>
+  </si>
+  <si>
+    <t>ma121</t>
+  </si>
+  <si>
+    <t>fasciola</t>
+  </si>
+  <si>
+    <t>ma246</t>
+  </si>
+  <si>
+    <t>teschovirus encephalomyelitis</t>
+  </si>
+  <si>
+    <t>ma415</t>
+  </si>
+  <si>
+    <t>helminthiasis</t>
+  </si>
+  <si>
+    <t>no_match_found</t>
+  </si>
+  <si>
+    <t>ma76</t>
+  </si>
+  <si>
+    <t>theileriases</t>
+  </si>
+  <si>
+    <t>nodavirus</t>
   </si>
 </sst>
 </file>
@@ -1923,7 +1962,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2103,6 +2142,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -2264,8 +2309,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2621,20 +2667,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E349"/>
+  <dimension ref="A1:F349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125:XFD125"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="34.6640625" customWidth="1"/>
     <col min="5" max="5" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2650,8 +2697,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2668,9 +2718,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -2685,7 +2735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2702,7 +2752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2719,7 +2769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2736,7 +2786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2753,7 +2803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2770,7 +2820,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2787,7 +2837,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2804,58 +2854,58 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>489</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>490</v>
+      </c>
+      <c r="D11" t="s">
         <v>491</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>492</v>
-      </c>
-      <c r="D11" t="s">
-        <v>493</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D12" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D13" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2872,7 +2922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -2889,7 +2939,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -2976,16 +3026,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>505</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>506</v>
+      </c>
+      <c r="D21" t="s">
         <v>507</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>508</v>
-      </c>
-      <c r="D21" t="s">
-        <v>509</v>
       </c>
       <c r="E21" t="s">
         <v>9</v>
@@ -2993,16 +3043,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>502</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>503</v>
+      </c>
+      <c r="D22" t="s">
         <v>504</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>505</v>
-      </c>
-      <c r="D22" t="s">
-        <v>506</v>
       </c>
       <c r="E22" t="s">
         <v>9</v>
@@ -3146,7 +3196,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -3163,7 +3213,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B32" t="s">
         <v>78</v>
@@ -5135,16 +5185,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B148" t="s">
         <v>6</v>
       </c>
       <c r="C148" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D148" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E148" t="s">
         <v>26</v>
@@ -6427,16 +6477,16 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
+        <v>584</v>
+      </c>
+      <c r="B224" t="s">
+        <v>6</v>
+      </c>
+      <c r="C224" t="s">
         <v>413</v>
       </c>
-      <c r="B224" t="s">
-        <v>6</v>
-      </c>
-      <c r="C224" t="s">
-        <v>414</v>
-      </c>
       <c r="D224" t="s">
-        <v>415</v>
+        <v>584</v>
       </c>
       <c r="E224" t="s">
         <v>26</v>
@@ -6444,16 +6494,16 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B225" t="s">
         <v>6</v>
       </c>
       <c r="C225" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D225" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E225" t="s">
         <v>26</v>
@@ -6461,16 +6511,16 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B226" t="s">
         <v>6</v>
       </c>
       <c r="C226" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D226" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E226" t="s">
         <v>26</v>
@@ -6478,16 +6528,16 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B227" t="s">
         <v>6</v>
       </c>
       <c r="C227" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D227" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E227" t="s">
         <v>26</v>
@@ -6495,16 +6545,16 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B228" t="s">
         <v>6</v>
       </c>
       <c r="C228" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D228" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E228" t="s">
         <v>26</v>
@@ -6512,16 +6562,16 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B229" t="s">
         <v>6</v>
       </c>
       <c r="C229" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D229" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E229" t="s">
         <v>26</v>
@@ -6529,16 +6579,16 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B230" t="s">
         <v>6</v>
       </c>
       <c r="C230" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D230" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E230" t="s">
         <v>26</v>
@@ -6546,16 +6596,16 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B231" t="s">
         <v>78</v>
       </c>
       <c r="C231" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D231" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E231" t="s">
         <v>26</v>
@@ -6563,16 +6613,16 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
+        <v>424</v>
+      </c>
+      <c r="B232" t="s">
+        <v>6</v>
+      </c>
+      <c r="C232" t="s">
+        <v>425</v>
+      </c>
+      <c r="D232" t="s">
         <v>426</v>
-      </c>
-      <c r="B232" t="s">
-        <v>6</v>
-      </c>
-      <c r="C232" t="s">
-        <v>427</v>
-      </c>
-      <c r="D232" t="s">
-        <v>428</v>
       </c>
       <c r="E232" t="s">
         <v>26</v>
@@ -6580,16 +6630,16 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B233" t="s">
         <v>6</v>
       </c>
       <c r="C233" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D233" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E233" t="s">
         <v>26</v>
@@ -6597,16 +6647,16 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B234" t="s">
         <v>6</v>
       </c>
       <c r="C234" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D234" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E234" t="s">
         <v>26</v>
@@ -6614,16 +6664,16 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
+        <v>429</v>
+      </c>
+      <c r="B235" t="s">
+        <v>6</v>
+      </c>
+      <c r="C235" t="s">
+        <v>430</v>
+      </c>
+      <c r="D235" t="s">
         <v>431</v>
-      </c>
-      <c r="B235" t="s">
-        <v>6</v>
-      </c>
-      <c r="C235" t="s">
-        <v>432</v>
-      </c>
-      <c r="D235" t="s">
-        <v>433</v>
       </c>
       <c r="E235" t="s">
         <v>26</v>
@@ -6631,16 +6681,16 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B236" t="s">
         <v>6</v>
       </c>
       <c r="C236" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D236" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E236" t="s">
         <v>26</v>
@@ -6648,16 +6698,16 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B237" t="s">
         <v>6</v>
       </c>
       <c r="C237" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D237" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E237" t="s">
         <v>26</v>
@@ -6665,16 +6715,16 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B238" t="s">
         <v>6</v>
       </c>
       <c r="C238" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D238" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E238" t="s">
         <v>26</v>
@@ -6682,16 +6732,16 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B239" t="s">
         <v>78</v>
       </c>
       <c r="C239" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D239" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E239" t="s">
         <v>26</v>
@@ -6699,16 +6749,16 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
+        <v>436</v>
+      </c>
+      <c r="B240" t="s">
+        <v>6</v>
+      </c>
+      <c r="C240" t="s">
+        <v>437</v>
+      </c>
+      <c r="D240" t="s">
         <v>438</v>
-      </c>
-      <c r="B240" t="s">
-        <v>6</v>
-      </c>
-      <c r="C240" t="s">
-        <v>439</v>
-      </c>
-      <c r="D240" t="s">
-        <v>440</v>
       </c>
       <c r="E240" t="s">
         <v>26</v>
@@ -6716,16 +6766,16 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B241" t="s">
         <v>6</v>
       </c>
       <c r="C241" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D241" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E241" t="s">
         <v>26</v>
@@ -6733,16 +6783,16 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B242" t="s">
         <v>6</v>
       </c>
       <c r="C242" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D242" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E242" t="s">
         <v>26</v>
@@ -6750,16 +6800,16 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B243" t="s">
         <v>78</v>
       </c>
       <c r="C243" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D243" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E243" t="s">
         <v>26</v>
@@ -6767,16 +6817,16 @@
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
+        <v>442</v>
+      </c>
+      <c r="B244" t="s">
+        <v>6</v>
+      </c>
+      <c r="C244" t="s">
+        <v>443</v>
+      </c>
+      <c r="D244" t="s">
         <v>444</v>
-      </c>
-      <c r="B244" t="s">
-        <v>6</v>
-      </c>
-      <c r="C244" t="s">
-        <v>445</v>
-      </c>
-      <c r="D244" t="s">
-        <v>446</v>
       </c>
       <c r="E244" t="s">
         <v>26</v>
@@ -6784,16 +6834,16 @@
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B245" t="s">
         <v>6</v>
       </c>
       <c r="C245" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D245" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E245" t="s">
         <v>26</v>
@@ -6801,16 +6851,16 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
+        <v>447</v>
+      </c>
+      <c r="B246" t="s">
+        <v>6</v>
+      </c>
+      <c r="C246" t="s">
+        <v>448</v>
+      </c>
+      <c r="D246" t="s">
         <v>449</v>
-      </c>
-      <c r="B246" t="s">
-        <v>6</v>
-      </c>
-      <c r="C246" t="s">
-        <v>450</v>
-      </c>
-      <c r="D246" t="s">
-        <v>451</v>
       </c>
       <c r="E246" t="s">
         <v>26</v>
@@ -6818,16 +6868,16 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B247" t="s">
         <v>78</v>
       </c>
       <c r="C247" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D247" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E247" t="s">
         <v>26</v>
@@ -6835,16 +6885,16 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B248" t="s">
         <v>78</v>
       </c>
       <c r="C248" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D248" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E248" t="s">
         <v>26</v>
@@ -6852,16 +6902,16 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
+        <v>452</v>
+      </c>
+      <c r="B249" t="s">
+        <v>6</v>
+      </c>
+      <c r="C249" t="s">
+        <v>453</v>
+      </c>
+      <c r="D249" t="s">
         <v>454</v>
-      </c>
-      <c r="B249" t="s">
-        <v>6</v>
-      </c>
-      <c r="C249" t="s">
-        <v>455</v>
-      </c>
-      <c r="D249" t="s">
-        <v>456</v>
       </c>
       <c r="E249" t="s">
         <v>26</v>
@@ -6869,16 +6919,16 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B250" t="s">
         <v>6</v>
       </c>
       <c r="C250" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D250" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E250" t="s">
         <v>26</v>
@@ -6886,16 +6936,16 @@
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B251" t="s">
         <v>6</v>
       </c>
       <c r="C251" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D251" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E251" t="s">
         <v>26</v>
@@ -6903,16 +6953,16 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B252" t="s">
         <v>78</v>
       </c>
       <c r="C252" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D252" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E252" t="s">
         <v>26</v>
@@ -6920,16 +6970,16 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
+        <v>459</v>
+      </c>
+      <c r="B253" t="s">
+        <v>6</v>
+      </c>
+      <c r="C253" t="s">
+        <v>460</v>
+      </c>
+      <c r="D253" t="s">
         <v>461</v>
-      </c>
-      <c r="B253" t="s">
-        <v>6</v>
-      </c>
-      <c r="C253" t="s">
-        <v>462</v>
-      </c>
-      <c r="D253" t="s">
-        <v>463</v>
       </c>
       <c r="E253" t="s">
         <v>26</v>
@@ -6937,16 +6987,16 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B254" t="s">
         <v>6</v>
       </c>
       <c r="C254" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D254" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E254" t="s">
         <v>26</v>
@@ -6954,16 +7004,16 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B255" t="s">
         <v>78</v>
       </c>
       <c r="C255" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D255" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E255" t="s">
         <v>26</v>
@@ -6971,16 +7021,16 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
+        <v>462</v>
+      </c>
+      <c r="B256" t="s">
+        <v>6</v>
+      </c>
+      <c r="C256" t="s">
+        <v>463</v>
+      </c>
+      <c r="D256" t="s">
         <v>464</v>
-      </c>
-      <c r="B256" t="s">
-        <v>6</v>
-      </c>
-      <c r="C256" t="s">
-        <v>465</v>
-      </c>
-      <c r="D256" t="s">
-        <v>466</v>
       </c>
       <c r="E256" t="s">
         <v>26</v>
@@ -6988,16 +7038,16 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B257" t="s">
         <v>6</v>
       </c>
       <c r="C257" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D257" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E257" t="s">
         <v>26</v>
@@ -7005,16 +7055,16 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B258" t="s">
         <v>78</v>
       </c>
       <c r="C258" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D258" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E258" t="s">
         <v>26</v>
@@ -7022,16 +7072,16 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
+        <v>466</v>
+      </c>
+      <c r="B259" t="s">
+        <v>6</v>
+      </c>
+      <c r="C259" t="s">
+        <v>467</v>
+      </c>
+      <c r="D259" t="s">
         <v>468</v>
-      </c>
-      <c r="B259" t="s">
-        <v>6</v>
-      </c>
-      <c r="C259" t="s">
-        <v>469</v>
-      </c>
-      <c r="D259" t="s">
-        <v>470</v>
       </c>
       <c r="E259" t="s">
         <v>26</v>
@@ -7039,16 +7089,16 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B260" t="s">
         <v>78</v>
       </c>
       <c r="C260" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D260" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E260" t="s">
         <v>26</v>
@@ -7056,16 +7106,16 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B261" t="s">
         <v>6</v>
       </c>
       <c r="C261" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D261" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E261" t="s">
         <v>26</v>
@@ -7073,16 +7123,16 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B262" t="s">
         <v>6</v>
       </c>
       <c r="C262" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D262" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E262" t="s">
         <v>26</v>
@@ -7090,16 +7140,16 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B263" t="s">
         <v>6</v>
       </c>
       <c r="C263" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D263" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E263" t="s">
         <v>26</v>
@@ -7107,16 +7157,16 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
+        <v>473</v>
+      </c>
+      <c r="B264" t="s">
+        <v>6</v>
+      </c>
+      <c r="C264" t="s">
+        <v>474</v>
+      </c>
+      <c r="D264" t="s">
         <v>475</v>
-      </c>
-      <c r="B264" t="s">
-        <v>6</v>
-      </c>
-      <c r="C264" t="s">
-        <v>476</v>
-      </c>
-      <c r="D264" t="s">
-        <v>477</v>
       </c>
       <c r="E264" t="s">
         <v>26</v>
@@ -7124,16 +7174,16 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B265" t="s">
         <v>78</v>
       </c>
       <c r="C265" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D265" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E265" t="s">
         <v>26</v>
@@ -7141,16 +7191,16 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B266" t="s">
         <v>6</v>
       </c>
       <c r="C266" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D266" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E266" t="s">
         <v>26</v>
@@ -7158,16 +7208,16 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B267" t="s">
         <v>6</v>
       </c>
       <c r="C267" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D267" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E267" t="s">
         <v>26</v>
@@ -7175,16 +7225,16 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
+        <v>480</v>
+      </c>
+      <c r="B268" t="s">
+        <v>6</v>
+      </c>
+      <c r="C268" t="s">
+        <v>481</v>
+      </c>
+      <c r="D268" t="s">
         <v>482</v>
-      </c>
-      <c r="B268" t="s">
-        <v>6</v>
-      </c>
-      <c r="C268" t="s">
-        <v>483</v>
-      </c>
-      <c r="D268" t="s">
-        <v>484</v>
       </c>
       <c r="E268" t="s">
         <v>26</v>
@@ -7192,7 +7242,7 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B269" t="s">
         <v>6</v>
@@ -7209,16 +7259,16 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B270" t="s">
         <v>6</v>
       </c>
       <c r="C270" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D270" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E270" t="s">
         <v>26</v>
@@ -7226,7 +7276,7 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>490</v>
+        <v>508</v>
       </c>
       <c r="B271" t="s">
         <v>6</v>
@@ -7243,58 +7293,58 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
+        <v>497</v>
+      </c>
+      <c r="B272" t="s">
+        <v>6</v>
+      </c>
+      <c r="C272" t="s">
+        <v>498</v>
+      </c>
+      <c r="D272" t="s">
         <v>499</v>
       </c>
-      <c r="B272" t="s">
-        <v>6</v>
-      </c>
-      <c r="C272" t="s">
+      <c r="E272" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
         <v>500</v>
       </c>
-      <c r="D272" t="s">
+      <c r="B273" t="s">
+        <v>6</v>
+      </c>
+      <c r="C273" t="s">
+        <v>498</v>
+      </c>
+      <c r="D273" t="s">
+        <v>499</v>
+      </c>
+      <c r="E273" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
         <v>501</v>
       </c>
-      <c r="E272" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A273" t="s">
-        <v>502</v>
-      </c>
-      <c r="B273" t="s">
-        <v>6</v>
-      </c>
-      <c r="C273" t="s">
-        <v>500</v>
-      </c>
-      <c r="D273" t="s">
-        <v>501</v>
-      </c>
-      <c r="E273" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A274" t="s">
-        <v>503</v>
-      </c>
       <c r="B274" t="s">
         <v>6</v>
       </c>
       <c r="C274" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D274" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E274" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A275" t="s">
-        <v>497</v>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A275" s="1" t="s">
+        <v>495</v>
       </c>
       <c r="B275" t="s">
         <v>78</v>
@@ -7308,130 +7358,139 @@
       <c r="E275" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F275" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
+        <v>509</v>
+      </c>
+      <c r="B276" t="s">
+        <v>6</v>
+      </c>
+      <c r="C276" t="s">
+        <v>62</v>
+      </c>
+      <c r="D276" t="s">
+        <v>62</v>
+      </c>
+      <c r="E276" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
         <v>510</v>
       </c>
-      <c r="B276" t="s">
-        <v>6</v>
-      </c>
-      <c r="C276" t="s">
-        <v>62</v>
-      </c>
-      <c r="D276" t="s">
-        <v>62</v>
-      </c>
-      <c r="E276" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A277" t="s">
+      <c r="B277" t="s">
+        <v>6</v>
+      </c>
+      <c r="C277" t="s">
+        <v>62</v>
+      </c>
+      <c r="D277" t="s">
+        <v>62</v>
+      </c>
+      <c r="E277" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
         <v>511</v>
       </c>
-      <c r="B277" t="s">
-        <v>6</v>
-      </c>
-      <c r="C277" t="s">
-        <v>62</v>
-      </c>
-      <c r="D277" t="s">
-        <v>62</v>
-      </c>
-      <c r="E277" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A278" t="s">
+      <c r="B278" t="s">
+        <v>6</v>
+      </c>
+      <c r="C278" t="s">
+        <v>62</v>
+      </c>
+      <c r="D278" t="s">
+        <v>62</v>
+      </c>
+      <c r="E278" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A279" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="B278" t="s">
-        <v>6</v>
-      </c>
-      <c r="C278" t="s">
-        <v>62</v>
-      </c>
-      <c r="D278" t="s">
-        <v>62</v>
-      </c>
-      <c r="E278" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A279" t="s">
+      <c r="B279" t="s">
+        <v>6</v>
+      </c>
+      <c r="C279" t="s">
+        <v>62</v>
+      </c>
+      <c r="D279" t="s">
+        <v>62</v>
+      </c>
+      <c r="E279" t="s">
+        <v>62</v>
+      </c>
+      <c r="F279" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
         <v>513</v>
       </c>
-      <c r="B279" t="s">
-        <v>6</v>
-      </c>
-      <c r="C279" t="s">
-        <v>62</v>
-      </c>
-      <c r="D279" t="s">
-        <v>62</v>
-      </c>
-      <c r="E279" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A280" t="s">
+      <c r="B280" t="s">
+        <v>6</v>
+      </c>
+      <c r="C280" t="s">
+        <v>585</v>
+      </c>
+      <c r="D280" t="s">
+        <v>586</v>
+      </c>
+      <c r="E280" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
         <v>514</v>
       </c>
-      <c r="B280" t="s">
-        <v>6</v>
-      </c>
-      <c r="C280" t="s">
-        <v>62</v>
-      </c>
-      <c r="D280" t="s">
-        <v>62</v>
-      </c>
-      <c r="E280" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A281" t="s">
+      <c r="B281" t="s">
+        <v>6</v>
+      </c>
+      <c r="C281" t="s">
+        <v>587</v>
+      </c>
+      <c r="D281" t="s">
+        <v>588</v>
+      </c>
+      <c r="E281" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A282" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="B281" t="s">
-        <v>6</v>
-      </c>
-      <c r="C281" t="s">
-        <v>62</v>
-      </c>
-      <c r="D281" t="s">
-        <v>62</v>
-      </c>
-      <c r="E281" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A282" t="s">
+      <c r="B282" t="s">
+        <v>6</v>
+      </c>
+      <c r="C282" t="s">
+        <v>62</v>
+      </c>
+      <c r="D282" t="s">
+        <v>62</v>
+      </c>
+      <c r="E282" t="s">
+        <v>62</v>
+      </c>
+      <c r="F282" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
         <v>516</v>
       </c>
-      <c r="B282" t="s">
-        <v>6</v>
-      </c>
-      <c r="C282" t="s">
-        <v>62</v>
-      </c>
-      <c r="D282" t="s">
-        <v>62</v>
-      </c>
-      <c r="E282" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A283" t="s">
-        <v>517</v>
-      </c>
       <c r="B283" t="s">
         <v>6</v>
       </c>
@@ -7445,9 +7504,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A284" t="s">
-        <v>517</v>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A284" s="1" t="s">
+        <v>515</v>
       </c>
       <c r="B284" t="s">
         <v>78</v>
@@ -7461,25 +7520,28 @@
       <c r="E284" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F284" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B285" t="s">
         <v>6</v>
       </c>
       <c r="C285" t="s">
-        <v>62</v>
+        <v>589</v>
       </c>
       <c r="D285" t="s">
-        <v>62</v>
+        <v>590</v>
       </c>
       <c r="E285" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>519</v>
       </c>
@@ -7487,18 +7549,18 @@
         <v>6</v>
       </c>
       <c r="C286" t="s">
-        <v>62</v>
+        <v>463</v>
       </c>
       <c r="D286" t="s">
-        <v>62</v>
+        <v>464</v>
       </c>
       <c r="E286" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A287" t="s">
-        <v>520</v>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A287" s="1" t="s">
+        <v>518</v>
       </c>
       <c r="B287" t="s">
         <v>78</v>
@@ -7512,127 +7574,136 @@
       <c r="E287" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F287" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
+        <v>520</v>
+      </c>
+      <c r="B288" t="s">
+        <v>6</v>
+      </c>
+      <c r="C288" t="s">
+        <v>463</v>
+      </c>
+      <c r="D288" t="s">
+        <v>464</v>
+      </c>
+      <c r="E288" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
         <v>521</v>
       </c>
-      <c r="B288" t="s">
-        <v>6</v>
-      </c>
-      <c r="C288" t="s">
-        <v>62</v>
-      </c>
-      <c r="D288" t="s">
-        <v>62</v>
-      </c>
-      <c r="E288" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A289" t="s">
+      <c r="B289" t="s">
+        <v>6</v>
+      </c>
+      <c r="C289" t="s">
+        <v>463</v>
+      </c>
+      <c r="D289" t="s">
+        <v>464</v>
+      </c>
+      <c r="E289" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
         <v>522</v>
       </c>
-      <c r="B289" t="s">
-        <v>6</v>
-      </c>
-      <c r="C289" t="s">
-        <v>62</v>
-      </c>
-      <c r="D289" t="s">
-        <v>62</v>
-      </c>
-      <c r="E289" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A290" t="s">
+      <c r="B290" t="s">
+        <v>6</v>
+      </c>
+      <c r="C290" t="s">
+        <v>591</v>
+      </c>
+      <c r="D290" t="s">
+        <v>592</v>
+      </c>
+      <c r="E290" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A291" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="B290" t="s">
-        <v>6</v>
-      </c>
-      <c r="C290" t="s">
-        <v>62</v>
-      </c>
-      <c r="D290" t="s">
-        <v>62</v>
-      </c>
-      <c r="E290" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A291" t="s">
+      <c r="B291" t="s">
+        <v>6</v>
+      </c>
+      <c r="C291" t="s">
+        <v>62</v>
+      </c>
+      <c r="D291" t="s">
+        <v>62</v>
+      </c>
+      <c r="E291" t="s">
+        <v>62</v>
+      </c>
+      <c r="F291" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
         <v>524</v>
       </c>
-      <c r="B291" t="s">
-        <v>6</v>
-      </c>
-      <c r="C291" t="s">
-        <v>62</v>
-      </c>
-      <c r="D291" t="s">
-        <v>62</v>
-      </c>
-      <c r="E291" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A292" t="s">
+      <c r="B292" t="s">
+        <v>6</v>
+      </c>
+      <c r="C292" t="s">
+        <v>61</v>
+      </c>
+      <c r="D292" t="s">
+        <v>61</v>
+      </c>
+      <c r="E292" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A293" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="B292" t="s">
-        <v>6</v>
-      </c>
-      <c r="C292" t="s">
-        <v>62</v>
-      </c>
-      <c r="D292" t="s">
-        <v>62</v>
-      </c>
-      <c r="E292" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A293" t="s">
+      <c r="B293" t="s">
+        <v>6</v>
+      </c>
+      <c r="C293" t="s">
+        <v>62</v>
+      </c>
+      <c r="D293" t="s">
+        <v>62</v>
+      </c>
+      <c r="E293" t="s">
+        <v>62</v>
+      </c>
+      <c r="F293" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
         <v>526</v>
       </c>
-      <c r="B293" t="s">
-        <v>6</v>
-      </c>
-      <c r="C293" t="s">
-        <v>62</v>
-      </c>
-      <c r="D293" t="s">
-        <v>62</v>
-      </c>
-      <c r="E293" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A294" t="s">
-        <v>527</v>
-      </c>
       <c r="B294" t="s">
         <v>6</v>
       </c>
       <c r="C294" t="s">
-        <v>62</v>
+        <v>593</v>
       </c>
       <c r="D294" t="s">
-        <v>62</v>
+        <v>594</v>
       </c>
       <c r="E294" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>528</v>
       </c>
@@ -7649,9 +7720,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A296" t="s">
-        <v>529</v>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A296" s="1" t="s">
+        <v>527</v>
       </c>
       <c r="B296" t="s">
         <v>78</v>
@@ -7665,300 +7736,330 @@
       <c r="E296" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F296" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
+        <v>529</v>
+      </c>
+      <c r="B297" t="s">
+        <v>6</v>
+      </c>
+      <c r="C297" t="s">
+        <v>62</v>
+      </c>
+      <c r="D297" t="s">
+        <v>62</v>
+      </c>
+      <c r="E297" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A298" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="B297" t="s">
-        <v>6</v>
-      </c>
-      <c r="C297" t="s">
-        <v>62</v>
-      </c>
-      <c r="D297" t="s">
-        <v>62</v>
-      </c>
-      <c r="E297" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A298" t="s">
+      <c r="B298" t="s">
+        <v>6</v>
+      </c>
+      <c r="C298" t="s">
+        <v>62</v>
+      </c>
+      <c r="D298" t="s">
+        <v>62</v>
+      </c>
+      <c r="E298" t="s">
+        <v>62</v>
+      </c>
+      <c r="F298" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A299" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="B298" t="s">
-        <v>6</v>
-      </c>
-      <c r="C298" t="s">
-        <v>62</v>
-      </c>
-      <c r="D298" t="s">
-        <v>62</v>
-      </c>
-      <c r="E298" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A299" t="s">
+      <c r="B299" t="s">
+        <v>6</v>
+      </c>
+      <c r="C299" t="s">
+        <v>62</v>
+      </c>
+      <c r="D299" t="s">
+        <v>62</v>
+      </c>
+      <c r="E299" t="s">
+        <v>62</v>
+      </c>
+      <c r="F299" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A300" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="B299" t="s">
-        <v>6</v>
-      </c>
-      <c r="C299" t="s">
-        <v>62</v>
-      </c>
-      <c r="D299" t="s">
-        <v>62</v>
-      </c>
-      <c r="E299" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A300" t="s">
+      <c r="B300" t="s">
+        <v>6</v>
+      </c>
+      <c r="C300" t="s">
+        <v>62</v>
+      </c>
+      <c r="D300" t="s">
+        <v>62</v>
+      </c>
+      <c r="E300" t="s">
+        <v>62</v>
+      </c>
+      <c r="F300" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A301" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="B300" t="s">
-        <v>6</v>
-      </c>
-      <c r="C300" t="s">
-        <v>62</v>
-      </c>
-      <c r="D300" t="s">
-        <v>62</v>
-      </c>
-      <c r="E300" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A301" t="s">
+      <c r="B301" t="s">
+        <v>6</v>
+      </c>
+      <c r="C301" t="s">
+        <v>62</v>
+      </c>
+      <c r="D301" t="s">
+        <v>62</v>
+      </c>
+      <c r="E301" t="s">
+        <v>62</v>
+      </c>
+      <c r="F301" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A302" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="B301" t="s">
-        <v>6</v>
-      </c>
-      <c r="C301" t="s">
-        <v>62</v>
-      </c>
-      <c r="D301" t="s">
-        <v>62</v>
-      </c>
-      <c r="E301" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A302" t="s">
+      <c r="B302" t="s">
+        <v>6</v>
+      </c>
+      <c r="C302" t="s">
+        <v>62</v>
+      </c>
+      <c r="D302" t="s">
+        <v>62</v>
+      </c>
+      <c r="E302" t="s">
+        <v>62</v>
+      </c>
+      <c r="F302" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A303" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="B302" t="s">
-        <v>6</v>
-      </c>
-      <c r="C302" t="s">
-        <v>62</v>
-      </c>
-      <c r="D302" t="s">
-        <v>62</v>
-      </c>
-      <c r="E302" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A303" t="s">
+      <c r="B303" t="s">
+        <v>6</v>
+      </c>
+      <c r="C303" t="s">
+        <v>62</v>
+      </c>
+      <c r="D303" t="s">
+        <v>62</v>
+      </c>
+      <c r="E303" t="s">
+        <v>62</v>
+      </c>
+      <c r="F303" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A304" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="B303" t="s">
-        <v>6</v>
-      </c>
-      <c r="C303" t="s">
-        <v>62</v>
-      </c>
-      <c r="D303" t="s">
-        <v>62</v>
-      </c>
-      <c r="E303" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A304" t="s">
+      <c r="B304" t="s">
+        <v>6</v>
+      </c>
+      <c r="C304" t="s">
+        <v>62</v>
+      </c>
+      <c r="D304" t="s">
+        <v>62</v>
+      </c>
+      <c r="E304" t="s">
+        <v>62</v>
+      </c>
+      <c r="F304" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A305" t="s">
         <v>537</v>
       </c>
-      <c r="B304" t="s">
-        <v>6</v>
-      </c>
-      <c r="C304" t="s">
-        <v>62</v>
-      </c>
-      <c r="D304" t="s">
-        <v>62</v>
-      </c>
-      <c r="E304" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A305" t="s">
+      <c r="B305" t="s">
+        <v>6</v>
+      </c>
+      <c r="C305" t="s">
+        <v>62</v>
+      </c>
+      <c r="D305" t="s">
+        <v>62</v>
+      </c>
+      <c r="E305" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A306" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="B305" t="s">
-        <v>6</v>
-      </c>
-      <c r="C305" t="s">
-        <v>62</v>
-      </c>
-      <c r="D305" t="s">
-        <v>62</v>
-      </c>
-      <c r="E305" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A306" t="s">
+      <c r="B306" t="s">
+        <v>6</v>
+      </c>
+      <c r="C306" t="s">
+        <v>62</v>
+      </c>
+      <c r="D306" t="s">
+        <v>62</v>
+      </c>
+      <c r="E306" t="s">
+        <v>62</v>
+      </c>
+      <c r="F306" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A307" t="s">
         <v>539</v>
       </c>
-      <c r="B306" t="s">
-        <v>6</v>
-      </c>
-      <c r="C306" t="s">
-        <v>62</v>
-      </c>
-      <c r="D306" t="s">
-        <v>62</v>
-      </c>
-      <c r="E306" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A307" t="s">
+      <c r="B307" t="s">
+        <v>6</v>
+      </c>
+      <c r="C307" t="s">
+        <v>62</v>
+      </c>
+      <c r="D307" t="s">
+        <v>62</v>
+      </c>
+      <c r="E307" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A308" t="s">
         <v>540</v>
       </c>
-      <c r="B307" t="s">
-        <v>6</v>
-      </c>
-      <c r="C307" t="s">
-        <v>62</v>
-      </c>
-      <c r="D307" t="s">
-        <v>62</v>
-      </c>
-      <c r="E307" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A308" t="s">
+      <c r="B308" t="s">
+        <v>6</v>
+      </c>
+      <c r="C308" t="s">
+        <v>62</v>
+      </c>
+      <c r="D308" t="s">
+        <v>62</v>
+      </c>
+      <c r="E308" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A309" t="s">
         <v>541</v>
       </c>
-      <c r="B308" t="s">
-        <v>6</v>
-      </c>
-      <c r="C308" t="s">
-        <v>62</v>
-      </c>
-      <c r="D308" t="s">
-        <v>62</v>
-      </c>
-      <c r="E308" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A309" t="s">
+      <c r="B309" t="s">
+        <v>6</v>
+      </c>
+      <c r="C309" t="s">
+        <v>62</v>
+      </c>
+      <c r="D309" t="s">
+        <v>62</v>
+      </c>
+      <c r="E309" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A310" t="s">
         <v>542</v>
       </c>
-      <c r="B309" t="s">
-        <v>6</v>
-      </c>
-      <c r="C309" t="s">
-        <v>62</v>
-      </c>
-      <c r="D309" t="s">
-        <v>62</v>
-      </c>
-      <c r="E309" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A310" t="s">
+      <c r="B310" t="s">
+        <v>6</v>
+      </c>
+      <c r="C310" t="s">
+        <v>62</v>
+      </c>
+      <c r="D310" t="s">
+        <v>62</v>
+      </c>
+      <c r="E310" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A311" t="s">
         <v>543</v>
       </c>
-      <c r="B310" t="s">
-        <v>6</v>
-      </c>
-      <c r="C310" t="s">
-        <v>62</v>
-      </c>
-      <c r="D310" t="s">
-        <v>62</v>
-      </c>
-      <c r="E310" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A311" t="s">
+      <c r="B311" t="s">
+        <v>6</v>
+      </c>
+      <c r="C311" t="s">
+        <v>62</v>
+      </c>
+      <c r="D311" t="s">
+        <v>62</v>
+      </c>
+      <c r="E311" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A312" t="s">
         <v>544</v>
       </c>
-      <c r="B311" t="s">
-        <v>6</v>
-      </c>
-      <c r="C311" t="s">
-        <v>62</v>
-      </c>
-      <c r="D311" t="s">
-        <v>62</v>
-      </c>
-      <c r="E311" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A312" t="s">
+      <c r="B312" t="s">
+        <v>6</v>
+      </c>
+      <c r="C312" t="s">
+        <v>62</v>
+      </c>
+      <c r="D312" t="s">
+        <v>62</v>
+      </c>
+      <c r="E312" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A313" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="B312" t="s">
-        <v>6</v>
-      </c>
-      <c r="C312" t="s">
-        <v>62</v>
-      </c>
-      <c r="D312" t="s">
-        <v>62</v>
-      </c>
-      <c r="E312" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A313" t="s">
+      <c r="B313" t="s">
+        <v>6</v>
+      </c>
+      <c r="C313" t="s">
+        <v>62</v>
+      </c>
+      <c r="D313" t="s">
+        <v>62</v>
+      </c>
+      <c r="E313" t="s">
+        <v>62</v>
+      </c>
+      <c r="F313" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A314" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="B313" t="s">
-        <v>6</v>
-      </c>
-      <c r="C313" t="s">
-        <v>62</v>
-      </c>
-      <c r="D313" t="s">
-        <v>62</v>
-      </c>
-      <c r="E313" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A314" t="s">
-        <v>547</v>
-      </c>
       <c r="B314" t="s">
         <v>6</v>
       </c>
@@ -7971,8 +8072,11 @@
       <c r="E314" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F314" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>548</v>
       </c>
@@ -7989,9 +8093,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A316" t="s">
-        <v>548</v>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A316" s="1" t="s">
+        <v>546</v>
       </c>
       <c r="B316" t="s">
         <v>78</v>
@@ -8005,10 +8109,13 @@
       <c r="E316" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A317" t="s">
-        <v>549</v>
+      <c r="F316" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A317" s="1" t="s">
+        <v>547</v>
       </c>
       <c r="B317" t="s">
         <v>78</v>
@@ -8022,44 +8129,47 @@
       <c r="E317" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F317" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
+        <v>549</v>
+      </c>
+      <c r="B318" t="s">
+        <v>6</v>
+      </c>
+      <c r="C318" t="s">
+        <v>62</v>
+      </c>
+      <c r="D318" t="s">
+        <v>62</v>
+      </c>
+      <c r="E318" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A319" t="s">
         <v>550</v>
       </c>
-      <c r="B318" t="s">
-        <v>6</v>
-      </c>
-      <c r="C318" t="s">
-        <v>62</v>
-      </c>
-      <c r="D318" t="s">
-        <v>62</v>
-      </c>
-      <c r="E318" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A319" t="s">
+      <c r="B319" t="s">
+        <v>6</v>
+      </c>
+      <c r="C319" t="s">
+        <v>62</v>
+      </c>
+      <c r="D319" t="s">
+        <v>62</v>
+      </c>
+      <c r="E319" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A320" t="s">
         <v>551</v>
-      </c>
-      <c r="B319" t="s">
-        <v>6</v>
-      </c>
-      <c r="C319" t="s">
-        <v>62</v>
-      </c>
-      <c r="D319" t="s">
-        <v>62</v>
-      </c>
-      <c r="E319" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A320" t="s">
-        <v>552</v>
       </c>
       <c r="B320" t="s">
         <v>6</v>
@@ -8076,7 +8186,7 @@
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B321" t="s">
         <v>6</v>
@@ -8093,7 +8203,7 @@
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B322" t="s">
         <v>6</v>
@@ -8110,7 +8220,7 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B323" t="s">
         <v>6</v>
@@ -8127,7 +8237,7 @@
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B324" t="s">
         <v>6</v>
@@ -8144,7 +8254,7 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B325" t="s">
         <v>6</v>
@@ -8161,7 +8271,7 @@
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B326" t="s">
         <v>6</v>
@@ -8178,7 +8288,7 @@
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B327" t="s">
         <v>6</v>
@@ -8195,7 +8305,7 @@
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B328" t="s">
         <v>6</v>
@@ -8212,7 +8322,7 @@
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B329" t="s">
         <v>6</v>
@@ -8229,7 +8339,7 @@
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B330" t="s">
         <v>6</v>
@@ -8246,7 +8356,7 @@
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B331" t="s">
         <v>6</v>
@@ -8263,7 +8373,7 @@
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B332" t="s">
         <v>6</v>
@@ -8280,7 +8390,7 @@
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B333" t="s">
         <v>6</v>
@@ -8297,7 +8407,7 @@
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B334" t="s">
         <v>6</v>
@@ -8314,7 +8424,7 @@
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B335" t="s">
         <v>6</v>
@@ -8331,248 +8441,247 @@
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
+        <v>567</v>
+      </c>
+      <c r="B336" t="s">
+        <v>6</v>
+      </c>
+      <c r="C336" t="s">
+        <v>62</v>
+      </c>
+      <c r="D336" t="s">
+        <v>62</v>
+      </c>
+      <c r="E336" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A337" t="s">
+        <v>488</v>
+      </c>
+      <c r="B337" t="s">
+        <v>6</v>
+      </c>
+      <c r="C337" t="s">
+        <v>596</v>
+      </c>
+      <c r="D337" t="s">
+        <v>597</v>
+      </c>
+      <c r="E337" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A338" t="s">
         <v>568</v>
       </c>
-      <c r="B336" t="s">
-        <v>6</v>
-      </c>
-      <c r="C336" t="s">
-        <v>62</v>
-      </c>
-      <c r="D336" t="s">
-        <v>62</v>
-      </c>
-      <c r="E336" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A337" t="s">
+      <c r="B338" t="s">
+        <v>6</v>
+      </c>
+      <c r="C338" t="s">
+        <v>62</v>
+      </c>
+      <c r="D338" t="s">
+        <v>62</v>
+      </c>
+      <c r="E338" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A339" t="s">
         <v>569</v>
       </c>
-      <c r="B337" t="s">
-        <v>6</v>
-      </c>
-      <c r="C337" t="s">
-        <v>62</v>
-      </c>
-      <c r="D337" t="s">
-        <v>62</v>
-      </c>
-      <c r="E337" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A338" t="s">
+      <c r="B339" t="s">
+        <v>6</v>
+      </c>
+      <c r="C339" t="s">
+        <v>62</v>
+      </c>
+      <c r="D339" t="s">
+        <v>62</v>
+      </c>
+      <c r="E339" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A340" t="s">
         <v>570</v>
       </c>
-      <c r="B338" t="s">
-        <v>6</v>
-      </c>
-      <c r="C338" t="s">
-        <v>62</v>
-      </c>
-      <c r="D338" t="s">
-        <v>62</v>
-      </c>
-      <c r="E338" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A339" t="s">
+      <c r="B340" t="s">
+        <v>6</v>
+      </c>
+      <c r="C340" t="s">
+        <v>62</v>
+      </c>
+      <c r="D340" t="s">
+        <v>62</v>
+      </c>
+      <c r="E340" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A341" t="s">
         <v>571</v>
       </c>
-      <c r="B339" t="s">
-        <v>6</v>
-      </c>
-      <c r="C339" t="s">
-        <v>62</v>
-      </c>
-      <c r="D339" t="s">
-        <v>62</v>
-      </c>
-      <c r="E339" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A340" t="s">
+      <c r="B341" t="s">
+        <v>6</v>
+      </c>
+      <c r="C341" t="s">
+        <v>62</v>
+      </c>
+      <c r="D341" t="s">
+        <v>62</v>
+      </c>
+      <c r="E341" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A342" t="s">
         <v>572</v>
-      </c>
-      <c r="B340" t="s">
-        <v>6</v>
-      </c>
-      <c r="C340" t="s">
-        <v>62</v>
-      </c>
-      <c r="D340" t="s">
-        <v>62</v>
-      </c>
-      <c r="E340" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A341" t="s">
-        <v>573</v>
-      </c>
-      <c r="B341" t="s">
-        <v>6</v>
-      </c>
-      <c r="C341" t="s">
-        <v>62</v>
-      </c>
-      <c r="D341" t="s">
-        <v>62</v>
-      </c>
-      <c r="E341" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A342" t="s">
-        <v>574</v>
       </c>
       <c r="B342" t="s">
         <v>78</v>
       </c>
       <c r="C342" t="s">
-        <v>62</v>
+        <v>214</v>
       </c>
       <c r="D342" t="s">
-        <v>62</v>
+        <v>213</v>
       </c>
       <c r="E342" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
+        <v>573</v>
+      </c>
+      <c r="B343" t="s">
+        <v>6</v>
+      </c>
+      <c r="C343" t="s">
+        <v>62</v>
+      </c>
+      <c r="D343" t="s">
+        <v>62</v>
+      </c>
+      <c r="E343" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A344" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B344" t="s">
+        <v>6</v>
+      </c>
+      <c r="C344" t="s">
+        <v>62</v>
+      </c>
+      <c r="D344" t="s">
+        <v>62</v>
+      </c>
+      <c r="E344" t="s">
+        <v>62</v>
+      </c>
+      <c r="F344" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A345" t="s">
         <v>575</v>
       </c>
-      <c r="B343" t="s">
-        <v>6</v>
-      </c>
-      <c r="C343" t="s">
-        <v>62</v>
-      </c>
-      <c r="D343" t="s">
-        <v>62</v>
-      </c>
-      <c r="E343" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A344" t="s">
+      <c r="B345" t="s">
+        <v>6</v>
+      </c>
+      <c r="C345" t="s">
+        <v>598</v>
+      </c>
+      <c r="D345" t="s">
+        <v>598</v>
+      </c>
+      <c r="E345" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A346" t="s">
         <v>576</v>
       </c>
-      <c r="B344" t="s">
-        <v>6</v>
-      </c>
-      <c r="C344" t="s">
-        <v>62</v>
-      </c>
-      <c r="D344" t="s">
-        <v>62</v>
-      </c>
-      <c r="E344" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A345" t="s">
+      <c r="B346" t="s">
+        <v>6</v>
+      </c>
+      <c r="C346" t="s">
         <v>577</v>
       </c>
-      <c r="B345" t="s">
-        <v>6</v>
-      </c>
-      <c r="C345" t="s">
-        <v>62</v>
-      </c>
-      <c r="D345" t="s">
-        <v>62</v>
-      </c>
-      <c r="E345" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A346" t="s">
-        <v>578</v>
-      </c>
-      <c r="B346" t="s">
-        <v>6</v>
-      </c>
-      <c r="C346" t="s">
-        <v>579</v>
-      </c>
       <c r="D346" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E346" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B347" t="s">
         <v>78</v>
       </c>
       <c r="C347" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D347" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E347" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B348" t="s">
         <v>78</v>
       </c>
       <c r="C348" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D348" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E348" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B349" t="s">
         <v>6</v>
       </c>
       <c r="C349" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D349" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E349" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{87BD2402-63CE-F446-9D6A-248EB5443D4B}">
-    <sortState ref="A2:E349">
-      <sortCondition ref="C1:C349"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:F349" xr:uid="{4FD3E36A-1C1B-A348-8C2F-386339E3FCC4}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove semicolon separated disease names
</commit_message>
<xml_diff>
--- a/inst/diseases/disease_lookup.xlsx
+++ b/inst/diseases/disease_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmamendelsohn/r_projects/wahis/inst/diseases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA61A22-1326-FC4A-BE5F-ED568C549F36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F76770D-A44E-5D49-92BA-0FE66C4A9258}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="-21140" windowWidth="20400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8400" yWindow="460" windowWidth="20400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="disease_lookup" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="606">
   <si>
     <t>disease</t>
   </si>
@@ -1432,9 +1432,6 @@
     <t>equine encephalomyelitis (eastern and western)</t>
   </si>
   <si>
-    <t>ma91;ma92</t>
-  </si>
-  <si>
     <t>equine encephalomyelitis (eastern andwestern)</t>
   </si>
   <si>
@@ -1759,9 +1756,6 @@
     <t>monkey pox</t>
   </si>
   <si>
-    <t>eastern equine encephalitis;western equine encephalitis</t>
-  </si>
-  <si>
     <t>ovine bluetongue disease</t>
   </si>
   <si>
@@ -1844,6 +1838,9 @@
   </si>
   <si>
     <t>oyster herpesvirus (oshv-1, mu var)</t>
+  </si>
+  <si>
+    <t>equine encephalitis</t>
   </si>
 </sst>
 </file>
@@ -2381,24 +2378,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2711,7 +2691,7 @@
   <dimension ref="A1:F351"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A352" sqref="A352"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2739,12 +2719,12 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
@@ -2764,7 +2744,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -2784,7 +2764,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2804,7 +2784,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B5" t="s">
         <v>77</v>
@@ -2824,7 +2804,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B6" t="s">
         <v>77</v>
@@ -2844,7 +2824,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -2864,7 +2844,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -2884,7 +2864,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B9" t="s">
         <v>77</v>
@@ -2904,7 +2884,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -2913,7 +2893,7 @@
         <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E10" t="s">
         <v>62</v>
@@ -2924,7 +2904,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -2933,7 +2913,7 @@
         <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E11" t="s">
         <v>62</v>
@@ -2944,7 +2924,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -2953,7 +2933,7 @@
         <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E12" t="s">
         <v>62</v>
@@ -2964,7 +2944,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -2973,7 +2953,7 @@
         <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E13" t="s">
         <v>62</v>
@@ -2984,7 +2964,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -3004,7 +2984,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -3024,7 +3004,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -3044,7 +3024,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -3053,7 +3033,7 @@
         <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E17" t="s">
         <v>62</v>
@@ -3064,7 +3044,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -3084,7 +3064,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -3104,7 +3084,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -3124,7 +3104,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B21" t="s">
         <v>77</v>
@@ -3144,7 +3124,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B22" t="s">
         <v>77</v>
@@ -3164,16 +3144,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
         <v>564</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" t="s">
-        <v>565</v>
       </c>
       <c r="E23" t="s">
         <v>62</v>
@@ -3184,7 +3164,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -3193,7 +3173,7 @@
         <v>62</v>
       </c>
       <c r="D24" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E24" t="s">
         <v>62</v>
@@ -3204,7 +3184,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -3213,7 +3193,7 @@
         <v>62</v>
       </c>
       <c r="D25" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E25" t="s">
         <v>62</v>
@@ -3224,7 +3204,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -3233,7 +3213,7 @@
         <v>62</v>
       </c>
       <c r="D26" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E26" t="s">
         <v>62</v>
@@ -3244,7 +3224,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
@@ -3281,7 +3261,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -3417,16 +3397,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>487</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
         <v>488</v>
       </c>
-      <c r="B37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>489</v>
-      </c>
-      <c r="D37" t="s">
-        <v>490</v>
       </c>
       <c r="E37" t="s">
         <v>9</v>
@@ -3434,16 +3414,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
       </c>
       <c r="C38" t="s">
+        <v>488</v>
+      </c>
+      <c r="D38" t="s">
         <v>489</v>
-      </c>
-      <c r="D38" t="s">
-        <v>490</v>
       </c>
       <c r="E38" t="s">
         <v>9</v>
@@ -3451,16 +3431,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
+        <v>488</v>
+      </c>
+      <c r="D39" t="s">
         <v>489</v>
-      </c>
-      <c r="D39" t="s">
-        <v>490</v>
       </c>
       <c r="E39" t="s">
         <v>9</v>
@@ -3587,16 +3567,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>503</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" t="s">
         <v>504</v>
       </c>
-      <c r="B47" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>505</v>
-      </c>
-      <c r="D47" t="s">
-        <v>506</v>
       </c>
       <c r="E47" t="s">
         <v>9</v>
@@ -3604,16 +3584,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>500</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
         <v>501</v>
       </c>
-      <c r="B48" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>502</v>
-      </c>
-      <c r="D48" t="s">
-        <v>503</v>
       </c>
       <c r="E48" t="s">
         <v>9</v>
@@ -3757,7 +3737,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B57" t="s">
         <v>6</v>
@@ -3774,7 +3754,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B58" t="s">
         <v>77</v>
@@ -3876,7 +3856,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B64" t="s">
         <v>6</v>
@@ -5746,16 +5726,16 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B174" t="s">
         <v>6</v>
       </c>
       <c r="C174" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D174" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E174" t="s">
         <v>26</v>
@@ -7038,7 +7018,7 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B250" t="s">
         <v>6</v>
@@ -7047,7 +7027,7 @@
         <v>412</v>
       </c>
       <c r="D250" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E250" t="s">
         <v>26</v>
@@ -7427,7 +7407,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>449</v>
       </c>
@@ -7444,7 +7424,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>450</v>
       </c>
@@ -7461,7 +7441,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>451</v>
       </c>
@@ -7478,7 +7458,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>454</v>
       </c>
@@ -7495,7 +7475,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>456</v>
       </c>
@@ -7512,7 +7492,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>456</v>
       </c>
@@ -7529,7 +7509,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>458</v>
       </c>
@@ -7546,9 +7526,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B280" t="s">
         <v>6</v>
@@ -7563,9 +7543,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B281" t="s">
         <v>77</v>
@@ -7580,7 +7560,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>461</v>
       </c>
@@ -7597,7 +7577,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>464</v>
       </c>
@@ -7614,7 +7594,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>464</v>
       </c>
@@ -7631,7 +7611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>465</v>
       </c>
@@ -7648,7 +7628,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>465</v>
       </c>
@@ -7665,145 +7645,154 @@
         <v>26</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A287" t="s">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A287" s="1" t="s">
         <v>468</v>
       </c>
       <c r="B287" t="s">
         <v>6</v>
       </c>
       <c r="C287" t="s">
+        <v>62</v>
+      </c>
+      <c r="D287" t="s">
+        <v>605</v>
+      </c>
+      <c r="E287" t="s">
+        <v>26</v>
+      </c>
+      <c r="F287" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A288" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="D287" t="s">
-        <v>578</v>
-      </c>
-      <c r="E287" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A288" t="s">
+      <c r="B288" t="s">
+        <v>6</v>
+      </c>
+      <c r="C288" t="s">
+        <v>62</v>
+      </c>
+      <c r="D288" t="s">
+        <v>605</v>
+      </c>
+      <c r="E288" t="s">
+        <v>26</v>
+      </c>
+      <c r="F288" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A289" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B288" t="s">
-        <v>6</v>
-      </c>
-      <c r="C288" t="s">
-        <v>469</v>
-      </c>
-      <c r="D288" t="s">
-        <v>578</v>
-      </c>
-      <c r="E288" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A289" t="s">
+      <c r="B289" t="s">
+        <v>6</v>
+      </c>
+      <c r="C289" t="s">
+        <v>62</v>
+      </c>
+      <c r="D289" t="s">
+        <v>605</v>
+      </c>
+      <c r="E289" t="s">
+        <v>26</v>
+      </c>
+      <c r="F289" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
         <v>471</v>
       </c>
-      <c r="B289" t="s">
-        <v>6</v>
-      </c>
-      <c r="C289" t="s">
-        <v>469</v>
-      </c>
-      <c r="D289" t="s">
-        <v>578</v>
-      </c>
-      <c r="E289" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A290" t="s">
+      <c r="B290" t="s">
+        <v>6</v>
+      </c>
+      <c r="C290" t="s">
         <v>472</v>
       </c>
-      <c r="B290" t="s">
-        <v>6</v>
-      </c>
-      <c r="C290" t="s">
+      <c r="D290" t="s">
         <v>473</v>
       </c>
-      <c r="D290" t="s">
-        <v>474</v>
-      </c>
       <c r="E290" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B291" t="s">
         <v>77</v>
       </c>
       <c r="C291" t="s">
+        <v>472</v>
+      </c>
+      <c r="D291" t="s">
         <v>473</v>
       </c>
-      <c r="D291" t="s">
+      <c r="E291" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
         <v>474</v>
       </c>
-      <c r="E291" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A292" t="s">
+      <c r="B292" t="s">
+        <v>6</v>
+      </c>
+      <c r="C292" t="s">
         <v>475</v>
       </c>
-      <c r="B292" t="s">
-        <v>6</v>
-      </c>
-      <c r="C292" t="s">
+      <c r="D292" t="s">
+        <v>474</v>
+      </c>
+      <c r="E292" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
         <v>476</v>
       </c>
-      <c r="D292" t="s">
-        <v>475</v>
-      </c>
-      <c r="E292" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A293" t="s">
+      <c r="B293" t="s">
+        <v>6</v>
+      </c>
+      <c r="C293" t="s">
         <v>477</v>
       </c>
-      <c r="B293" t="s">
-        <v>6</v>
-      </c>
-      <c r="C293" t="s">
+      <c r="D293" t="s">
+        <v>476</v>
+      </c>
+      <c r="E293" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
         <v>478</v>
       </c>
-      <c r="D293" t="s">
-        <v>477</v>
-      </c>
-      <c r="E293" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A294" t="s">
+      <c r="B294" t="s">
+        <v>6</v>
+      </c>
+      <c r="C294" t="s">
         <v>479</v>
       </c>
-      <c r="B294" t="s">
-        <v>6</v>
-      </c>
-      <c r="C294" t="s">
+      <c r="D294" t="s">
         <v>480</v>
       </c>
-      <c r="D294" t="s">
+      <c r="E294" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A295" t="s">
         <v>481</v>
-      </c>
-      <c r="E294" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A295" t="s">
-        <v>482</v>
       </c>
       <c r="B295" t="s">
         <v>6</v>
@@ -7818,154 +7807,154 @@
         <v>26</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B296" t="s">
         <v>6</v>
       </c>
       <c r="C296" t="s">
+        <v>580</v>
+      </c>
+      <c r="D296" t="s">
+        <v>579</v>
+      </c>
+      <c r="E296" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A297" t="s">
+        <v>506</v>
+      </c>
+      <c r="B297" t="s">
+        <v>6</v>
+      </c>
+      <c r="C297" t="s">
+        <v>596</v>
+      </c>
+      <c r="D297" t="s">
+        <v>597</v>
+      </c>
+      <c r="E297" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A298" t="s">
+        <v>495</v>
+      </c>
+      <c r="B298" t="s">
+        <v>6</v>
+      </c>
+      <c r="C298" t="s">
+        <v>496</v>
+      </c>
+      <c r="D298" t="s">
+        <v>497</v>
+      </c>
+      <c r="E298" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
+        <v>498</v>
+      </c>
+      <c r="B299" t="s">
+        <v>6</v>
+      </c>
+      <c r="C299" t="s">
+        <v>496</v>
+      </c>
+      <c r="D299" t="s">
+        <v>497</v>
+      </c>
+      <c r="E299" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A300" t="s">
+        <v>499</v>
+      </c>
+      <c r="B300" t="s">
+        <v>6</v>
+      </c>
+      <c r="C300" t="s">
+        <v>496</v>
+      </c>
+      <c r="D300" t="s">
+        <v>497</v>
+      </c>
+      <c r="E300" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A301" t="s">
+        <v>507</v>
+      </c>
+      <c r="B301" t="s">
+        <v>6</v>
+      </c>
+      <c r="C301" t="s">
+        <v>596</v>
+      </c>
+      <c r="D301" t="s">
+        <v>597</v>
+      </c>
+      <c r="E301" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A302" t="s">
+        <v>508</v>
+      </c>
+      <c r="B302" t="s">
+        <v>6</v>
+      </c>
+      <c r="C302" t="s">
+        <v>596</v>
+      </c>
+      <c r="D302" t="s">
+        <v>597</v>
+      </c>
+      <c r="E302" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A303" t="s">
+        <v>509</v>
+      </c>
+      <c r="B303" t="s">
+        <v>6</v>
+      </c>
+      <c r="C303" t="s">
+        <v>596</v>
+      </c>
+      <c r="D303" t="s">
+        <v>597</v>
+      </c>
+      <c r="E303" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A304" t="s">
+        <v>511</v>
+      </c>
+      <c r="B304" t="s">
+        <v>6</v>
+      </c>
+      <c r="C304" t="s">
         <v>582</v>
       </c>
-      <c r="D296" t="s">
-        <v>581</v>
-      </c>
-      <c r="E296" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A297" t="s">
-        <v>507</v>
-      </c>
-      <c r="B297" t="s">
-        <v>6</v>
-      </c>
-      <c r="C297" t="s">
-        <v>598</v>
-      </c>
-      <c r="D297" t="s">
-        <v>599</v>
-      </c>
-      <c r="E297" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A298" t="s">
-        <v>496</v>
-      </c>
-      <c r="B298" t="s">
-        <v>6</v>
-      </c>
-      <c r="C298" t="s">
-        <v>497</v>
-      </c>
-      <c r="D298" t="s">
-        <v>498</v>
-      </c>
-      <c r="E298" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A299" t="s">
-        <v>499</v>
-      </c>
-      <c r="B299" t="s">
-        <v>6</v>
-      </c>
-      <c r="C299" t="s">
-        <v>497</v>
-      </c>
-      <c r="D299" t="s">
-        <v>498</v>
-      </c>
-      <c r="E299" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A300" t="s">
-        <v>500</v>
-      </c>
-      <c r="B300" t="s">
-        <v>6</v>
-      </c>
-      <c r="C300" t="s">
-        <v>497</v>
-      </c>
-      <c r="D300" t="s">
-        <v>498</v>
-      </c>
-      <c r="E300" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A301" t="s">
-        <v>508</v>
-      </c>
-      <c r="B301" t="s">
-        <v>6</v>
-      </c>
-      <c r="C301" t="s">
-        <v>598</v>
-      </c>
-      <c r="D301" t="s">
-        <v>599</v>
-      </c>
-      <c r="E301" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A302" t="s">
-        <v>509</v>
-      </c>
-      <c r="B302" t="s">
-        <v>6</v>
-      </c>
-      <c r="C302" t="s">
-        <v>598</v>
-      </c>
-      <c r="D302" t="s">
-        <v>599</v>
-      </c>
-      <c r="E302" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A303" t="s">
-        <v>510</v>
-      </c>
-      <c r="B303" t="s">
-        <v>6</v>
-      </c>
-      <c r="C303" t="s">
-        <v>598</v>
-      </c>
-      <c r="D303" t="s">
-        <v>599</v>
-      </c>
-      <c r="E303" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A304" t="s">
-        <v>512</v>
-      </c>
-      <c r="B304" t="s">
-        <v>6</v>
-      </c>
-      <c r="C304" t="s">
-        <v>584</v>
-      </c>
       <c r="D304" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E304" t="s">
         <v>9</v>
@@ -7973,16 +7962,16 @@
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B305" t="s">
         <v>6</v>
       </c>
       <c r="C305" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D305" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E305" t="s">
         <v>26</v>
@@ -7990,7 +7979,7 @@
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B306" t="s">
         <v>6</v>
@@ -8007,16 +7996,16 @@
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B307" t="s">
         <v>6</v>
       </c>
       <c r="C307" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D307" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E307" t="s">
         <v>26</v>
@@ -8024,7 +8013,7 @@
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B308" t="s">
         <v>6</v>
@@ -8041,7 +8030,7 @@
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B309" t="s">
         <v>6</v>
@@ -8058,7 +8047,7 @@
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B310" t="s">
         <v>6</v>
@@ -8075,16 +8064,16 @@
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B311" t="s">
         <v>6</v>
       </c>
       <c r="C311" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D311" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E311" t="s">
         <v>26</v>
@@ -8092,7 +8081,7 @@
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B312" t="s">
         <v>6</v>
@@ -8109,16 +8098,16 @@
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B313" t="s">
         <v>6</v>
       </c>
       <c r="C313" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D313" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E313" t="s">
         <v>26</v>
@@ -8126,7 +8115,7 @@
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A314" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B314" t="s">
         <v>6</v>
@@ -8146,7 +8135,7 @@
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B315" t="s">
         <v>6</v>
@@ -8163,13 +8152,13 @@
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B316" t="s">
         <v>6</v>
       </c>
       <c r="C316" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D316" t="s">
         <v>62</v>
@@ -8180,16 +8169,16 @@
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B317" t="s">
         <v>6</v>
       </c>
       <c r="C317" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D317" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E317" t="s">
         <v>26</v>
@@ -8197,16 +8186,16 @@
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B318" t="s">
         <v>6</v>
       </c>
       <c r="C318" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D318" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E318" t="s">
         <v>26</v>
@@ -8214,16 +8203,16 @@
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B319" t="s">
         <v>6</v>
       </c>
       <c r="C319" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D319" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E319" t="s">
         <v>26</v>
@@ -8231,16 +8220,16 @@
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B320" t="s">
         <v>6</v>
       </c>
       <c r="C320" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D320" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E320" t="s">
         <v>26</v>
@@ -8248,13 +8237,13 @@
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A321" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B321" t="s">
         <v>6</v>
       </c>
       <c r="C321" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D321" t="s">
         <v>62</v>
@@ -8268,7 +8257,7 @@
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B322" t="s">
         <v>6</v>
@@ -8288,7 +8277,7 @@
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A323" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B323" t="s">
         <v>6</v>
@@ -8305,16 +8294,16 @@
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B324" t="s">
         <v>6</v>
       </c>
       <c r="C324" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D324" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E324" t="s">
         <v>26</v>
@@ -8322,16 +8311,16 @@
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B325" t="s">
         <v>6</v>
       </c>
       <c r="C325" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D325" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E325" t="s">
         <v>26</v>
@@ -8339,16 +8328,16 @@
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B326" t="s">
         <v>6</v>
       </c>
       <c r="C326" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D326" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E326" t="s">
         <v>26</v>
@@ -8356,16 +8345,16 @@
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B327" t="s">
         <v>6</v>
       </c>
       <c r="C327" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D327" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E327" t="s">
         <v>26</v>
@@ -8373,16 +8362,16 @@
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B328" t="s">
         <v>6</v>
       </c>
       <c r="C328" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D328" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E328" t="s">
         <v>26</v>
@@ -8390,16 +8379,16 @@
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B329" t="s">
         <v>6</v>
       </c>
       <c r="C329" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D329" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E329" t="s">
         <v>26</v>
@@ -8407,16 +8396,16 @@
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B330" t="s">
         <v>6</v>
       </c>
       <c r="C330" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D330" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E330" t="s">
         <v>26</v>
@@ -8424,16 +8413,16 @@
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B331" t="s">
         <v>6</v>
       </c>
       <c r="C331" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D331" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E331" t="s">
         <v>26</v>
@@ -8441,16 +8430,16 @@
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B332" t="s">
         <v>6</v>
       </c>
       <c r="C332" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D332" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E332" t="s">
         <v>26</v>
@@ -8458,16 +8447,16 @@
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B333" t="s">
         <v>6</v>
       </c>
       <c r="C333" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D333" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E333" t="s">
         <v>26</v>
@@ -8475,16 +8464,16 @@
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B334" t="s">
         <v>6</v>
       </c>
       <c r="C334" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D334" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E334" t="s">
         <v>26</v>
@@ -8492,16 +8481,16 @@
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B335" t="s">
         <v>6</v>
       </c>
       <c r="C335" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D335" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E335" t="s">
         <v>26</v>
@@ -8509,16 +8498,16 @@
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B336" t="s">
         <v>6</v>
       </c>
       <c r="C336" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D336" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E336" t="s">
         <v>26</v>
@@ -8526,7 +8515,7 @@
     </row>
     <row r="337" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A337" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B337" t="s">
         <v>6</v>
@@ -8546,16 +8535,16 @@
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B338" t="s">
         <v>6</v>
       </c>
       <c r="C338" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D338" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E338" t="s">
         <v>26</v>
@@ -8563,16 +8552,16 @@
     </row>
     <row r="339" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B339" t="s">
         <v>6</v>
       </c>
       <c r="C339" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D339" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E339" t="s">
         <v>26</v>
@@ -8580,7 +8569,7 @@
     </row>
     <row r="340" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B340" t="s">
         <v>6</v>
@@ -8589,7 +8578,7 @@
         <v>62</v>
       </c>
       <c r="D340" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E340" t="s">
         <v>62</v>
@@ -8600,7 +8589,7 @@
     </row>
     <row r="341" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A341" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B341" t="s">
         <v>6</v>
@@ -8609,7 +8598,7 @@
         <v>62</v>
       </c>
       <c r="D341" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E341" t="s">
         <v>62</v>
@@ -8620,7 +8609,7 @@
     </row>
     <row r="342" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A342" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B342" t="s">
         <v>6</v>
@@ -8629,7 +8618,7 @@
         <v>62</v>
       </c>
       <c r="D342" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E342" t="s">
         <v>62</v>
@@ -8640,7 +8629,7 @@
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A343" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B343" t="s">
         <v>6</v>
@@ -8649,7 +8638,7 @@
         <v>62</v>
       </c>
       <c r="D343" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E343" t="s">
         <v>62</v>
@@ -8660,7 +8649,7 @@
     </row>
     <row r="344" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B344" t="s">
         <v>77</v>
@@ -8677,16 +8666,16 @@
     </row>
     <row r="345" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B345" t="s">
         <v>6</v>
       </c>
       <c r="C345" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="D345" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E345" t="s">
         <v>9</v>
@@ -8694,16 +8683,16 @@
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
+        <v>574</v>
+      </c>
+      <c r="B346" t="s">
+        <v>6</v>
+      </c>
+      <c r="C346" t="s">
         <v>575</v>
       </c>
-      <c r="B346" t="s">
-        <v>6</v>
-      </c>
-      <c r="C346" t="s">
-        <v>576</v>
-      </c>
       <c r="D346" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E346" t="s">
         <v>9</v>
@@ -8711,16 +8700,16 @@
     </row>
     <row r="347" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B347" t="s">
         <v>77</v>
       </c>
       <c r="C347" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D347" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E347" t="s">
         <v>9</v>
@@ -8728,16 +8717,16 @@
     </row>
     <row r="348" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B348" t="s">
         <v>77</v>
       </c>
       <c r="C348" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D348" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E348" t="s">
         <v>9</v>
@@ -8745,16 +8734,16 @@
     </row>
     <row r="349" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B349" t="s">
         <v>6</v>
       </c>
       <c r="C349" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D349" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E349" t="s">
         <v>9</v>
@@ -8762,16 +8751,16 @@
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B350" t="s">
         <v>6</v>
       </c>
       <c r="C350" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D350" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E350" t="s">
         <v>26</v>
@@ -8779,7 +8768,7 @@
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A351" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B351" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
add missing disease group
</commit_message>
<xml_diff>
--- a/inst/diseases/disease_lookup.xlsx
+++ b/inst/diseases/disease_lookup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmamendelsohn/r_projects/wahis/inst/diseases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D78AEDF-201B-AB41-A95B-2BE8E8C7E0E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BF2C02-CDC5-664E-935E-7C5369F9CEC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7060" yWindow="460" windowWidth="20400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2692,11 +2692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F351"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C353" sqref="C353"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2727,7 +2726,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>491</v>
       </c>
@@ -2747,7 +2746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>508</v>
       </c>
@@ -2767,7 +2766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>511</v>
       </c>
@@ -2787,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>511</v>
       </c>
@@ -2807,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>514</v>
       </c>
@@ -2827,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>519</v>
       </c>
@@ -2847,7 +2846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>521</v>
       </c>
@@ -2867,7 +2866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>523</v>
       </c>
@@ -2887,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>526</v>
       </c>
@@ -2907,7 +2906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>527</v>
       </c>
@@ -2927,7 +2926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>528</v>
       </c>
@@ -2947,7 +2946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>529</v>
       </c>
@@ -2967,7 +2966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>530</v>
       </c>
@@ -2987,7 +2986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>531</v>
       </c>
@@ -3007,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>532</v>
       </c>
@@ -3027,7 +3026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>533</v>
       </c>
@@ -3047,7 +3046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>534</v>
       </c>
@@ -3067,7 +3066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>541</v>
       </c>
@@ -3087,7 +3086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>542</v>
       </c>
@@ -3107,7 +3106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>542</v>
       </c>
@@ -3127,7 +3126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>543</v>
       </c>
@@ -3147,7 +3146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>561</v>
       </c>
@@ -3167,7 +3166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>562</v>
       </c>
@@ -3187,7 +3186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>563</v>
       </c>
@@ -3207,7 +3206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>569</v>
       </c>
@@ -3227,7 +3226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>570</v>
       </c>
@@ -3247,7 +3246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>466</v>
       </c>
@@ -3267,7 +3266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>467</v>
       </c>
@@ -3287,7 +3286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>468</v>
       </c>
@@ -3307,7 +3306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>524</v>
       </c>
@@ -3327,7 +3326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>540</v>
       </c>
@@ -3347,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>544</v>
       </c>
@@ -3367,7 +3366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>545</v>
       </c>
@@ -3384,7 +3383,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>559</v>
       </c>
@@ -3404,7 +3403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>564</v>
       </c>
@@ -3424,7 +3423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>565</v>
       </c>
@@ -3444,7 +3443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>566</v>
       </c>
@@ -3464,7 +3463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>567</v>
       </c>
@@ -3484,7 +3483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>601</v>
       </c>
@@ -3504,7 +3503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -3521,7 +3520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>490</v>
       </c>
@@ -3538,7 +3537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -3555,7 +3554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -3572,7 +3571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -3589,7 +3588,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -3606,7 +3605,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -3623,7 +3622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>27</v>
       </c>
@@ -3640,7 +3639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -3657,7 +3656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>485</v>
       </c>
@@ -3674,7 +3673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>488</v>
       </c>
@@ -3691,7 +3690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>489</v>
       </c>
@@ -3708,7 +3707,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -3725,7 +3724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>34</v>
       </c>
@@ -3742,7 +3741,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -3759,7 +3758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>40</v>
       </c>
@@ -3776,7 +3775,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -3793,7 +3792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>46</v>
       </c>
@@ -3810,7 +3809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>47</v>
       </c>
@@ -3827,7 +3826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>501</v>
       </c>
@@ -3844,7 +3843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>498</v>
       </c>
@@ -3878,7 +3877,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>49</v>
       </c>
@@ -3895,7 +3894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>52</v>
       </c>
@@ -3912,7 +3911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>53</v>
       </c>
@@ -3929,7 +3928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>54</v>
       </c>
@@ -3946,7 +3945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>55</v>
       </c>
@@ -3963,7 +3962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>57</v>
       </c>
@@ -3980,7 +3979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>58</v>
       </c>
@@ -3997,7 +3996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>492</v>
       </c>
@@ -4014,7 +4013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>492</v>
       </c>
@@ -4031,7 +4030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>59</v>
       </c>
@@ -4048,7 +4047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>62</v>
       </c>
@@ -4065,7 +4064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>63</v>
       </c>
@@ -4082,7 +4081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>64</v>
       </c>
@@ -4099,7 +4098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>65</v>
       </c>
@@ -4116,7 +4115,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>602</v>
       </c>
@@ -4133,7 +4132,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>66</v>
       </c>
@@ -4150,7 +4149,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>67</v>
       </c>
@@ -4167,7 +4166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>68</v>
       </c>
@@ -4184,7 +4183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>69</v>
       </c>
@@ -4201,7 +4200,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>72</v>
       </c>
@@ -4218,7 +4217,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>74</v>
       </c>
@@ -4235,7 +4234,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>74</v>
       </c>
@@ -4252,7 +4251,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>77</v>
       </c>
@@ -4269,7 +4268,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>79</v>
       </c>
@@ -4286,7 +4285,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>82</v>
       </c>
@@ -4303,7 +4302,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>85</v>
       </c>
@@ -4320,7 +4319,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -4337,7 +4336,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -4354,7 +4353,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -4371,7 +4370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>93</v>
       </c>
@@ -4388,7 +4387,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -4405,7 +4404,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>95</v>
       </c>
@@ -4422,7 +4421,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>98</v>
       </c>
@@ -4439,7 +4438,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>100</v>
       </c>
@@ -4456,7 +4455,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>100</v>
       </c>
@@ -4473,7 +4472,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>103</v>
       </c>
@@ -4490,7 +4489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>104</v>
       </c>
@@ -4507,7 +4506,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>105</v>
       </c>
@@ -4524,7 +4523,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>106</v>
       </c>
@@ -4541,7 +4540,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>106</v>
       </c>
@@ -4558,7 +4557,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>108</v>
       </c>
@@ -4575,7 +4574,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>111</v>
       </c>
@@ -4592,7 +4591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>113</v>
       </c>
@@ -4609,7 +4608,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>113</v>
       </c>
@@ -4626,7 +4625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>115</v>
       </c>
@@ -4643,7 +4642,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>118</v>
       </c>
@@ -4660,7 +4659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>120</v>
       </c>
@@ -4677,7 +4676,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>123</v>
       </c>
@@ -4694,7 +4693,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>125</v>
       </c>
@@ -4711,7 +4710,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>126</v>
       </c>
@@ -4728,7 +4727,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>127</v>
       </c>
@@ -4745,7 +4744,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>130</v>
       </c>
@@ -4762,7 +4761,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>131</v>
       </c>
@@ -4779,7 +4778,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>132</v>
       </c>
@@ -4796,7 +4795,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>134</v>
       </c>
@@ -4813,7 +4812,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>136</v>
       </c>
@@ -4830,7 +4829,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>138</v>
       </c>
@@ -4847,7 +4846,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>139</v>
       </c>
@@ -4864,7 +4863,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>140</v>
       </c>
@@ -4881,7 +4880,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>143</v>
       </c>
@@ -4898,7 +4897,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>146</v>
       </c>
@@ -4915,7 +4914,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>148</v>
       </c>
@@ -4932,7 +4931,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>151</v>
       </c>
@@ -4949,7 +4948,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>152</v>
       </c>
@@ -4966,7 +4965,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>155</v>
       </c>
@@ -4983,7 +4982,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>158</v>
       </c>
@@ -5000,7 +4999,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>161</v>
       </c>
@@ -5017,7 +5016,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>164</v>
       </c>
@@ -5034,7 +5033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>165</v>
       </c>
@@ -5051,7 +5050,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>165</v>
       </c>
@@ -5068,7 +5067,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>166</v>
       </c>
@@ -5085,7 +5084,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>167</v>
       </c>
@@ -5102,7 +5101,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>167</v>
       </c>
@@ -5119,7 +5118,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>168</v>
       </c>
@@ -5136,7 +5135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>170</v>
       </c>
@@ -5153,7 +5152,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>172</v>
       </c>
@@ -5170,7 +5169,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>174</v>
       </c>
@@ -5187,7 +5186,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>176</v>
       </c>
@@ -5204,7 +5203,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>179</v>
       </c>
@@ -5221,7 +5220,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>182</v>
       </c>
@@ -5238,7 +5237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>185</v>
       </c>
@@ -5255,7 +5254,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>188</v>
       </c>
@@ -5272,7 +5271,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>191</v>
       </c>
@@ -5289,7 +5288,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>193</v>
       </c>
@@ -5306,7 +5305,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>194</v>
       </c>
@@ -5323,7 +5322,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>195</v>
       </c>
@@ -5340,7 +5339,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>198</v>
       </c>
@@ -5357,7 +5356,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>199</v>
       </c>
@@ -5374,7 +5373,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>201</v>
       </c>
@@ -5391,7 +5390,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>204</v>
       </c>
@@ -5408,7 +5407,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>205</v>
       </c>
@@ -5425,7 +5424,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>208</v>
       </c>
@@ -5442,7 +5441,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>209</v>
       </c>
@@ -5459,7 +5458,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>210</v>
       </c>
@@ -5476,7 +5475,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>211</v>
       </c>
@@ -5493,7 +5492,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>213</v>
       </c>
@@ -5527,7 +5526,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>218</v>
       </c>
@@ -5544,7 +5543,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>221</v>
       </c>
@@ -5561,7 +5560,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>221</v>
       </c>
@@ -5578,7 +5577,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>224</v>
       </c>
@@ -5595,7 +5594,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>227</v>
       </c>
@@ -5612,7 +5611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>229</v>
       </c>
@@ -5629,7 +5628,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>231</v>
       </c>
@@ -5646,7 +5645,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>233</v>
       </c>
@@ -5663,7 +5662,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>235</v>
       </c>
@@ -5680,7 +5679,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>238</v>
       </c>
@@ -5697,7 +5696,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>241</v>
       </c>
@@ -5714,7 +5713,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>241</v>
       </c>
@@ -5731,7 +5730,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>243</v>
       </c>
@@ -5748,7 +5747,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>245</v>
       </c>
@@ -5765,7 +5764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>246</v>
       </c>
@@ -5782,7 +5781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>247</v>
       </c>
@@ -5799,7 +5798,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>250</v>
       </c>
@@ -5816,7 +5815,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>252</v>
       </c>
@@ -5833,7 +5832,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>254</v>
       </c>
@@ -5850,7 +5849,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>256</v>
       </c>
@@ -5867,7 +5866,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>257</v>
       </c>
@@ -5884,7 +5883,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>259</v>
       </c>
@@ -5901,7 +5900,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>262</v>
       </c>
@@ -5918,7 +5917,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>264</v>
       </c>
@@ -5935,7 +5934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>267</v>
       </c>
@@ -5952,7 +5951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>269</v>
       </c>
@@ -5969,7 +5968,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="186" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>482</v>
       </c>
@@ -5986,7 +5985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>270</v>
       </c>
@@ -6003,7 +6002,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>272</v>
       </c>
@@ -6020,7 +6019,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>273</v>
       </c>
@@ -6037,7 +6036,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>275</v>
       </c>
@@ -6054,7 +6053,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>276</v>
       </c>
@@ -6071,7 +6070,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="192" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>277</v>
       </c>
@@ -6088,7 +6087,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>280</v>
       </c>
@@ -6105,7 +6104,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>283</v>
       </c>
@@ -6122,7 +6121,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>283</v>
       </c>
@@ -6139,7 +6138,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>285</v>
       </c>
@@ -6156,7 +6155,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>285</v>
       </c>
@@ -6173,7 +6172,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>287</v>
       </c>
@@ -6190,7 +6189,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>290</v>
       </c>
@@ -6207,7 +6206,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>293</v>
       </c>
@@ -6224,7 +6223,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>294</v>
       </c>
@@ -6241,7 +6240,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>294</v>
       </c>
@@ -6258,7 +6257,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>23</v>
       </c>
@@ -6275,7 +6274,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>296</v>
       </c>
@@ -6292,7 +6291,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>299</v>
       </c>
@@ -6309,7 +6308,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>302</v>
       </c>
@@ -6326,7 +6325,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>304</v>
       </c>
@@ -6343,7 +6342,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>307</v>
       </c>
@@ -6360,7 +6359,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>308</v>
       </c>
@@ -6377,7 +6376,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>311</v>
       </c>
@@ -6394,7 +6393,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>312</v>
       </c>
@@ -6411,7 +6410,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>315</v>
       </c>
@@ -6428,7 +6427,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>316</v>
       </c>
@@ -6445,7 +6444,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>317</v>
       </c>
@@ -6462,7 +6461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>318</v>
       </c>
@@ -6479,7 +6478,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>321</v>
       </c>
@@ -6496,7 +6495,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>324</v>
       </c>
@@ -6513,7 +6512,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>325</v>
       </c>
@@ -6530,7 +6529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>328</v>
       </c>
@@ -6547,7 +6546,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>331</v>
       </c>
@@ -6564,7 +6563,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="221" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>332</v>
       </c>
@@ -6581,7 +6580,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>335</v>
       </c>
@@ -6598,7 +6597,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>336</v>
       </c>
@@ -6615,7 +6614,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>338</v>
       </c>
@@ -6632,7 +6631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>340</v>
       </c>
@@ -6649,7 +6648,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>343</v>
       </c>
@@ -6666,7 +6665,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>344</v>
       </c>
@@ -6683,7 +6682,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>345</v>
       </c>
@@ -6700,7 +6699,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>346</v>
       </c>
@@ -6717,7 +6716,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>348</v>
       </c>
@@ -6734,7 +6733,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>350</v>
       </c>
@@ -6751,7 +6750,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>353</v>
       </c>
@@ -6768,7 +6767,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>354</v>
       </c>
@@ -6785,7 +6784,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>356</v>
       </c>
@@ -6802,7 +6801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>359</v>
       </c>
@@ -6819,7 +6818,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>361</v>
       </c>
@@ -6836,7 +6835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>364</v>
       </c>
@@ -6853,7 +6852,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>367</v>
       </c>
@@ -6870,7 +6869,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>370</v>
       </c>
@@ -6887,7 +6886,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>373</v>
       </c>
@@ -6904,7 +6903,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>373</v>
       </c>
@@ -6921,7 +6920,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="242" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>374</v>
       </c>
@@ -6938,7 +6937,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="243" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>375</v>
       </c>
@@ -6955,7 +6954,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="244" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>376</v>
       </c>
@@ -6972,7 +6971,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="245" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>377</v>
       </c>
@@ -6989,7 +6988,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="246" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>377</v>
       </c>
@@ -7006,7 +7005,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="247" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>379</v>
       </c>
@@ -7023,7 +7022,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="248" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>381</v>
       </c>
@@ -7040,7 +7039,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="249" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>382</v>
       </c>
@@ -7057,7 +7056,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="250" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>384</v>
       </c>
@@ -7074,7 +7073,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="251" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>386</v>
       </c>
@@ -7091,7 +7090,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="252" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>389</v>
       </c>
@@ -7108,7 +7107,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="253" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>390</v>
       </c>
@@ -7125,7 +7124,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="254" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>391</v>
       </c>
@@ -7142,7 +7141,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="255" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>394</v>
       </c>
@@ -7159,7 +7158,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="256" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>397</v>
       </c>
@@ -7176,7 +7175,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="257" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>399</v>
       </c>
@@ -7193,7 +7192,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="258" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>401</v>
       </c>
@@ -7210,7 +7209,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="259" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>403</v>
       </c>
@@ -7227,7 +7226,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="260" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>405</v>
       </c>
@@ -7244,7 +7243,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="261" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>407</v>
       </c>
@@ -7261,7 +7260,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>579</v>
       </c>
@@ -7278,7 +7277,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="263" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>411</v>
       </c>
@@ -7295,7 +7294,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="264" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>413</v>
       </c>
@@ -7312,7 +7311,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="265" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>414</v>
       </c>
@@ -7329,7 +7328,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>415</v>
       </c>
@@ -7346,7 +7345,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>417</v>
       </c>
@@ -7363,7 +7362,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="268" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>419</v>
       </c>
@@ -7380,7 +7379,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="269" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>419</v>
       </c>
@@ -7397,7 +7396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="270" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>421</v>
       </c>
@@ -7414,7 +7413,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="271" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>424</v>
       </c>
@@ -7431,7 +7430,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="272" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>425</v>
       </c>
@@ -7448,7 +7447,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>426</v>
       </c>
@@ -7465,7 +7464,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="274" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>429</v>
       </c>
@@ -7482,7 +7481,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="275" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>430</v>
       </c>
@@ -7499,7 +7498,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="276" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>431</v>
       </c>
@@ -7516,7 +7515,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="277" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>432</v>
       </c>
@@ -7533,7 +7532,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>433</v>
       </c>
@@ -7550,7 +7549,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>436</v>
       </c>
@@ -7567,7 +7566,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="280" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>437</v>
       </c>
@@ -7584,7 +7583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="281" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>437</v>
       </c>
@@ -7601,7 +7600,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>439</v>
       </c>
@@ -7618,7 +7617,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="283" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>442</v>
       </c>
@@ -7635,7 +7634,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="284" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>444</v>
       </c>
@@ -7652,7 +7651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="285" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>447</v>
       </c>
@@ -7669,7 +7668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="286" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>448</v>
       </c>
@@ -7686,7 +7685,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>449</v>
       </c>
@@ -7703,7 +7702,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>452</v>
       </c>
@@ -7720,7 +7719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="289" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>454</v>
       </c>
@@ -7737,7 +7736,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="290" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>454</v>
       </c>
@@ -7754,7 +7753,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="291" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>456</v>
       </c>
@@ -7771,7 +7770,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="292" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>481</v>
       </c>
@@ -7788,7 +7787,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="293" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>481</v>
       </c>
@@ -7805,7 +7804,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="294" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>459</v>
       </c>
@@ -7822,7 +7821,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="295" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>462</v>
       </c>
@@ -7839,7 +7838,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="296" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>462</v>
       </c>
@@ -7856,7 +7855,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="297" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>463</v>
       </c>
@@ -7873,7 +7872,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="298" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>463</v>
       </c>
@@ -7890,7 +7889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="299" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>469</v>
       </c>
@@ -7907,7 +7906,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="300" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>469</v>
       </c>
@@ -7924,7 +7923,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="301" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>472</v>
       </c>
@@ -7941,7 +7940,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="302" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>474</v>
       </c>
@@ -7958,7 +7957,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="303" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>476</v>
       </c>
@@ -7975,7 +7974,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="304" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>479</v>
       </c>
@@ -7992,7 +7991,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>483</v>
       </c>
@@ -8009,7 +8008,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>504</v>
       </c>
@@ -8026,7 +8025,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>493</v>
       </c>
@@ -8043,7 +8042,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>496</v>
       </c>
@@ -8060,7 +8059,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>497</v>
       </c>
@@ -8077,7 +8076,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>505</v>
       </c>
@@ -8094,7 +8093,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>506</v>
       </c>
@@ -8111,7 +8110,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>507</v>
       </c>
@@ -8128,7 +8127,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>509</v>
       </c>
@@ -8145,7 +8144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>510</v>
       </c>
@@ -8162,7 +8161,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>512</v>
       </c>
@@ -8179,7 +8178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="316" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>513</v>
       </c>
@@ -8196,7 +8195,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>515</v>
       </c>
@@ -8210,10 +8209,10 @@
         <v>461</v>
       </c>
       <c r="E317" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>516</v>
       </c>
@@ -8230,7 +8229,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>517</v>
       </c>
@@ -8247,7 +8246,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>518</v>
       </c>
@@ -8264,7 +8263,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>520</v>
       </c>
@@ -8281,7 +8280,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>522</v>
       </c>
@@ -8298,7 +8297,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>525</v>
       </c>
@@ -8315,7 +8314,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>535</v>
       </c>
@@ -8332,7 +8331,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>536</v>
       </c>
@@ -8349,7 +8348,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="326" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>537</v>
       </c>
@@ -8366,7 +8365,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>538</v>
       </c>
@@ -8383,7 +8382,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="328" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>539</v>
       </c>
@@ -8400,7 +8399,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>546</v>
       </c>
@@ -8417,7 +8416,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>547</v>
       </c>
@@ -8434,7 +8433,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="331" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>548</v>
       </c>
@@ -8451,7 +8450,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="332" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>549</v>
       </c>
@@ -8468,7 +8467,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="333" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>550</v>
       </c>
@@ -8485,7 +8484,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="334" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>551</v>
       </c>
@@ -8502,7 +8501,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="335" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>552</v>
       </c>
@@ -8519,7 +8518,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="336" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>553</v>
       </c>
@@ -8536,7 +8535,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="337" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>554</v>
       </c>
@@ -8553,7 +8552,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="338" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>555</v>
       </c>
@@ -8570,7 +8569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="339" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>556</v>
       </c>
@@ -8587,7 +8586,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="340" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>557</v>
       </c>
@@ -8604,7 +8603,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="341" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>558</v>
       </c>
@@ -8621,7 +8620,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="342" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>560</v>
       </c>
@@ -8638,7 +8637,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="343" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>484</v>
       </c>
@@ -8655,7 +8654,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="344" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>568</v>
       </c>
@@ -8672,7 +8671,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="345" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>571</v>
       </c>
@@ -8689,7 +8688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="346" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>572</v>
       </c>
@@ -8706,7 +8705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="347" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>572</v>
       </c>
@@ -8723,7 +8722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="348" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>574</v>
       </c>
@@ -8740,7 +8739,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="349" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>574</v>
       </c>
@@ -8757,7 +8756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="350" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>504</v>
       </c>
@@ -8792,14 +8791,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F351" xr:uid="{4FD3E36A-1C1B-A348-8C2F-386339E3FCC4}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="porcine epidemic diarrhea"/>
-        <filter val="porcine epidemic diarrhea virus"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F351" xr:uid="{4FD3E36A-1C1B-A348-8C2F-386339E3FCC4}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Serotype and taxa population handling
</commit_message>
<xml_diff>
--- a/inst/diseases/disease_lookup.xlsx
+++ b/inst/diseases/disease_lookup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmamendelsohn/r_projects/wahis/inst/diseases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BF2C02-CDC5-664E-935E-7C5369F9CEC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A28DF6-BEF8-604C-8894-8194F24106B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7060" yWindow="460" windowWidth="20400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="604">
   <si>
     <t>disease</t>
   </si>
@@ -1138,12 +1138,6 @@
     <t>highly path. avian influenza</t>
   </si>
   <si>
-    <t>ma418</t>
-  </si>
-  <si>
-    <t>avian influenza</t>
-  </si>
-  <si>
     <t>highly pathogenic avian influenza</t>
   </si>
   <si>
@@ -1838,6 +1832,9 @@
   </si>
   <si>
     <t>virus de la diarrea epidemica porcina</t>
+  </si>
+  <si>
+    <t>low pathogenic avian influenza</t>
   </si>
 </sst>
 </file>
@@ -2694,13 +2691,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F351"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="E244" sqref="E244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="1" max="1" width="58.5" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="34.6640625" customWidth="1"/>
     <col min="5" max="5" width="33.1640625" customWidth="1"/>
@@ -2723,12 +2720,12 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B2" t="s">
         <v>76</v>
@@ -2748,7 +2745,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -2768,7 +2765,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2788,7 +2785,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B5" t="s">
         <v>76</v>
@@ -2808,7 +2805,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B6" t="s">
         <v>76</v>
@@ -2828,7 +2825,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -2848,7 +2845,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -2868,7 +2865,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B9" t="s">
         <v>76</v>
@@ -2888,7 +2885,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -2897,7 +2894,7 @@
         <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E10" t="s">
         <v>61</v>
@@ -2908,7 +2905,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -2917,7 +2914,7 @@
         <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E11" t="s">
         <v>61</v>
@@ -2928,7 +2925,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -2937,7 +2934,7 @@
         <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E12" t="s">
         <v>61</v>
@@ -2948,7 +2945,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -2957,7 +2954,7 @@
         <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E13" t="s">
         <v>61</v>
@@ -2968,7 +2965,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -2988,7 +2985,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -3008,7 +3005,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -3028,7 +3025,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -3037,7 +3034,7 @@
         <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E17" t="s">
         <v>61</v>
@@ -3048,7 +3045,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -3068,7 +3065,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -3088,7 +3085,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -3108,7 +3105,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B21" t="s">
         <v>76</v>
@@ -3128,7 +3125,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B22" t="s">
         <v>76</v>
@@ -3148,7 +3145,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -3157,7 +3154,7 @@
         <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E23" t="s">
         <v>61</v>
@@ -3168,7 +3165,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -3177,7 +3174,7 @@
         <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E24" t="s">
         <v>61</v>
@@ -3188,7 +3185,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -3197,7 +3194,7 @@
         <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E25" t="s">
         <v>61</v>
@@ -3208,7 +3205,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -3217,7 +3214,7 @@
         <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E26" t="s">
         <v>61</v>
@@ -3228,7 +3225,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
@@ -3248,7 +3245,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -3257,7 +3254,7 @@
         <v>61</v>
       </c>
       <c r="D28" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E28" t="s">
         <v>26</v>
@@ -3268,7 +3265,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -3277,7 +3274,7 @@
         <v>61</v>
       </c>
       <c r="D29" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E29" t="s">
         <v>26</v>
@@ -3288,7 +3285,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -3297,7 +3294,7 @@
         <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E30" t="s">
         <v>26</v>
@@ -3308,7 +3305,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -3328,13 +3325,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D32" t="s">
         <v>61</v>
@@ -3348,7 +3345,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -3368,7 +3365,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -3385,7 +3382,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -3405,7 +3402,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
@@ -3414,7 +3411,7 @@
         <v>61</v>
       </c>
       <c r="D36" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E36" t="s">
         <v>61</v>
@@ -3425,7 +3422,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
@@ -3434,7 +3431,7 @@
         <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E37" t="s">
         <v>61</v>
@@ -3445,7 +3442,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -3454,7 +3451,7 @@
         <v>61</v>
       </c>
       <c r="D38" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E38" t="s">
         <v>61</v>
@@ -3465,7 +3462,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -3474,7 +3471,7 @@
         <v>61</v>
       </c>
       <c r="D39" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E39" t="s">
         <v>61</v>
@@ -3485,7 +3482,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
@@ -3522,7 +3519,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
@@ -3658,16 +3655,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>483</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>484</v>
+      </c>
+      <c r="D50" t="s">
         <v>485</v>
-      </c>
-      <c r="B50" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" t="s">
-        <v>486</v>
-      </c>
-      <c r="D50" t="s">
-        <v>487</v>
       </c>
       <c r="E50" t="s">
         <v>9</v>
@@ -3675,16 +3672,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D51" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E51" t="s">
         <v>9</v>
@@ -3692,16 +3689,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D52" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E52" t="s">
         <v>9</v>
@@ -3828,16 +3825,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>499</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>500</v>
+      </c>
+      <c r="D60" t="s">
         <v>501</v>
-      </c>
-      <c r="B60" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" t="s">
-        <v>502</v>
-      </c>
-      <c r="D60" t="s">
-        <v>503</v>
       </c>
       <c r="E60" t="s">
         <v>9</v>
@@ -3845,16 +3842,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>496</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>497</v>
+      </c>
+      <c r="D61" t="s">
         <v>498</v>
-      </c>
-      <c r="B61" t="s">
-        <v>6</v>
-      </c>
-      <c r="C61" t="s">
-        <v>499</v>
-      </c>
-      <c r="D61" t="s">
-        <v>500</v>
       </c>
       <c r="E61" t="s">
         <v>9</v>
@@ -3998,7 +3995,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B70" t="s">
         <v>6</v>
@@ -4015,7 +4012,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B71" t="s">
         <v>76</v>
@@ -4117,7 +4114,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
@@ -5970,16 +5967,16 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B186" t="s">
         <v>6</v>
       </c>
       <c r="C186" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D186" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="E186" t="s">
         <v>26</v>
@@ -6631,7 +6628,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>340</v>
       </c>
@@ -6648,7 +6645,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>343</v>
       </c>
@@ -6665,7 +6662,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>344</v>
       </c>
@@ -6682,7 +6679,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>345</v>
       </c>
@@ -6699,7 +6696,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>346</v>
       </c>
@@ -6716,7 +6713,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>348</v>
       </c>
@@ -6733,7 +6730,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>350</v>
       </c>
@@ -6750,7 +6747,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>353</v>
       </c>
@@ -6767,7 +6764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>354</v>
       </c>
@@ -6784,7 +6781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>356</v>
       </c>
@@ -6801,7 +6798,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>359</v>
       </c>
@@ -6818,7 +6815,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>361</v>
       </c>
@@ -6835,7 +6832,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>364</v>
       </c>
@@ -6852,7 +6849,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>367</v>
       </c>
@@ -6869,7 +6866,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>370</v>
       </c>
@@ -6877,299 +6874,317 @@
         <v>6</v>
       </c>
       <c r="C239" t="s">
+        <v>61</v>
+      </c>
+      <c r="D239" t="s">
         <v>371</v>
       </c>
-      <c r="D239" t="s">
-        <v>372</v>
-      </c>
       <c r="E239" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="F239" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B240" t="s">
         <v>6</v>
       </c>
       <c r="C240" t="s">
+        <v>61</v>
+      </c>
+      <c r="D240" t="s">
         <v>371</v>
       </c>
-      <c r="D240" t="s">
-        <v>372</v>
-      </c>
       <c r="E240" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="F240" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B241" t="s">
         <v>76</v>
       </c>
       <c r="C241" t="s">
+        <v>61</v>
+      </c>
+      <c r="D241" t="s">
         <v>371</v>
       </c>
-      <c r="D241" t="s">
+      <c r="E241" t="s">
+        <v>61</v>
+      </c>
+      <c r="F241" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
         <v>372</v>
       </c>
-      <c r="E241" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A242" t="s">
+      <c r="B242" t="s">
+        <v>6</v>
+      </c>
+      <c r="C242" t="s">
+        <v>61</v>
+      </c>
+      <c r="D242" t="s">
+        <v>371</v>
+      </c>
+      <c r="E242" t="s">
+        <v>61</v>
+      </c>
+      <c r="F242" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>373</v>
+      </c>
+      <c r="B243" t="s">
+        <v>6</v>
+      </c>
+      <c r="C243" t="s">
+        <v>61</v>
+      </c>
+      <c r="D243" t="s">
+        <v>371</v>
+      </c>
+      <c r="E243" t="s">
+        <v>61</v>
+      </c>
+      <c r="F243" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
         <v>374</v>
       </c>
-      <c r="B242" t="s">
-        <v>6</v>
-      </c>
-      <c r="C242" t="s">
-        <v>371</v>
-      </c>
-      <c r="D242" t="s">
-        <v>372</v>
-      </c>
-      <c r="E242" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A243" t="s">
+      <c r="B244" t="s">
+        <v>6</v>
+      </c>
+      <c r="C244" t="s">
+        <v>61</v>
+      </c>
+      <c r="D244" t="s">
+        <v>603</v>
+      </c>
+      <c r="E244" t="s">
+        <v>61</v>
+      </c>
+      <c r="F244" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
         <v>375</v>
       </c>
-      <c r="B243" t="s">
-        <v>6</v>
-      </c>
-      <c r="C243" t="s">
-        <v>371</v>
-      </c>
-      <c r="D243" t="s">
-        <v>372</v>
-      </c>
-      <c r="E243" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A244" t="s">
+      <c r="B245" t="s">
+        <v>6</v>
+      </c>
+      <c r="C245" t="s">
         <v>376</v>
       </c>
-      <c r="B244" t="s">
-        <v>6</v>
-      </c>
-      <c r="C244" t="s">
-        <v>371</v>
-      </c>
-      <c r="D244" t="s">
-        <v>372</v>
-      </c>
-      <c r="E244" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A245" t="s">
-        <v>377</v>
-      </c>
-      <c r="B245" t="s">
-        <v>6</v>
-      </c>
-      <c r="C245" t="s">
-        <v>378</v>
-      </c>
       <c r="D245" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E245" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B246" t="s">
         <v>76</v>
       </c>
       <c r="C246" t="s">
+        <v>376</v>
+      </c>
+      <c r="D246" t="s">
+        <v>375</v>
+      </c>
+      <c r="E246" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>377</v>
+      </c>
+      <c r="B247" t="s">
+        <v>6</v>
+      </c>
+      <c r="C247" t="s">
         <v>378</v>
       </c>
-      <c r="D246" t="s">
-        <v>377</v>
-      </c>
-      <c r="E246" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A247" t="s">
+      <c r="D247" t="s">
         <v>379</v>
       </c>
-      <c r="B247" t="s">
-        <v>6</v>
-      </c>
-      <c r="C247" t="s">
+      <c r="E247" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>379</v>
+      </c>
+      <c r="B248" t="s">
+        <v>6</v>
+      </c>
+      <c r="C248" t="s">
+        <v>378</v>
+      </c>
+      <c r="D248" t="s">
+        <v>379</v>
+      </c>
+      <c r="E248" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
         <v>380</v>
       </c>
-      <c r="D247" t="s">
+      <c r="B249" t="s">
+        <v>6</v>
+      </c>
+      <c r="C249" t="s">
         <v>381</v>
       </c>
-      <c r="E247" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A248" t="s">
-        <v>381</v>
-      </c>
-      <c r="B248" t="s">
-        <v>6</v>
-      </c>
-      <c r="C248" t="s">
+      <c r="D249" t="s">
         <v>380</v>
       </c>
-      <c r="D248" t="s">
-        <v>381</v>
-      </c>
-      <c r="E248" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A249" t="s">
+      <c r="E249" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
         <v>382</v>
       </c>
-      <c r="B249" t="s">
-        <v>6</v>
-      </c>
-      <c r="C249" t="s">
+      <c r="B250" t="s">
+        <v>6</v>
+      </c>
+      <c r="C250" t="s">
         <v>383</v>
       </c>
-      <c r="D249" t="s">
+      <c r="D250" t="s">
         <v>382</v>
       </c>
-      <c r="E249" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A250" t="s">
+      <c r="E250" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
         <v>384</v>
       </c>
-      <c r="B250" t="s">
-        <v>6</v>
-      </c>
-      <c r="C250" t="s">
+      <c r="B251" t="s">
+        <v>6</v>
+      </c>
+      <c r="C251" t="s">
         <v>385</v>
       </c>
-      <c r="D250" t="s">
-        <v>384</v>
-      </c>
-      <c r="E250" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A251" t="s">
+      <c r="D251" t="s">
         <v>386</v>
       </c>
-      <c r="B251" t="s">
-        <v>6</v>
-      </c>
-      <c r="C251" t="s">
+      <c r="E251" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
         <v>387</v>
       </c>
-      <c r="D251" t="s">
+      <c r="B252" t="s">
+        <v>6</v>
+      </c>
+      <c r="C252" t="s">
+        <v>385</v>
+      </c>
+      <c r="D252" t="s">
+        <v>386</v>
+      </c>
+      <c r="E252" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
         <v>388</v>
       </c>
-      <c r="E251" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A252" t="s">
+      <c r="B253" t="s">
+        <v>6</v>
+      </c>
+      <c r="C253" t="s">
+        <v>385</v>
+      </c>
+      <c r="D253" t="s">
+        <v>386</v>
+      </c>
+      <c r="E253" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
         <v>389</v>
       </c>
-      <c r="B252" t="s">
-        <v>6</v>
-      </c>
-      <c r="C252" t="s">
-        <v>387</v>
-      </c>
-      <c r="D252" t="s">
-        <v>388</v>
-      </c>
-      <c r="E252" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A253" t="s">
+      <c r="B254" t="s">
+        <v>6</v>
+      </c>
+      <c r="C254" t="s">
         <v>390</v>
       </c>
-      <c r="B253" t="s">
-        <v>6</v>
-      </c>
-      <c r="C253" t="s">
-        <v>387</v>
-      </c>
-      <c r="D253" t="s">
-        <v>388</v>
-      </c>
-      <c r="E253" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A254" t="s">
+      <c r="D254" t="s">
         <v>391</v>
       </c>
-      <c r="B254" t="s">
-        <v>6</v>
-      </c>
-      <c r="C254" t="s">
+      <c r="E254" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
         <v>392</v>
       </c>
-      <c r="D254" t="s">
+      <c r="B255" t="s">
+        <v>6</v>
+      </c>
+      <c r="C255" t="s">
         <v>393</v>
       </c>
-      <c r="E254" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A255" t="s">
+      <c r="D255" t="s">
         <v>394</v>
       </c>
-      <c r="B255" t="s">
-        <v>6</v>
-      </c>
-      <c r="C255" t="s">
+      <c r="E255" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
         <v>395</v>
       </c>
-      <c r="D255" t="s">
+      <c r="B256" t="s">
+        <v>6</v>
+      </c>
+      <c r="C256" t="s">
         <v>396</v>
       </c>
-      <c r="E255" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A256" t="s">
-        <v>397</v>
-      </c>
-      <c r="B256" t="s">
-        <v>6</v>
-      </c>
-      <c r="C256" t="s">
-        <v>398</v>
-      </c>
       <c r="D256" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E256" t="s">
         <v>26</v>
@@ -7177,16 +7192,16 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B257" t="s">
         <v>6</v>
       </c>
       <c r="C257" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D257" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E257" t="s">
         <v>26</v>
@@ -7194,16 +7209,16 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B258" t="s">
         <v>6</v>
       </c>
       <c r="C258" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D258" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E258" t="s">
         <v>26</v>
@@ -7211,16 +7226,16 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B259" t="s">
         <v>6</v>
       </c>
       <c r="C259" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D259" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E259" t="s">
         <v>26</v>
@@ -7228,16 +7243,16 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B260" t="s">
         <v>6</v>
       </c>
       <c r="C260" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D260" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E260" t="s">
         <v>26</v>
@@ -7245,16 +7260,16 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
+        <v>405</v>
+      </c>
+      <c r="B261" t="s">
+        <v>6</v>
+      </c>
+      <c r="C261" t="s">
+        <v>406</v>
+      </c>
+      <c r="D261" t="s">
         <v>407</v>
-      </c>
-      <c r="B261" t="s">
-        <v>6</v>
-      </c>
-      <c r="C261" t="s">
-        <v>408</v>
-      </c>
-      <c r="D261" t="s">
-        <v>409</v>
       </c>
       <c r="E261" t="s">
         <v>26</v>
@@ -7262,16 +7277,16 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B262" t="s">
         <v>6</v>
       </c>
       <c r="C262" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D262" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E262" t="s">
         <v>26</v>
@@ -7279,16 +7294,16 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B263" t="s">
         <v>6</v>
       </c>
       <c r="C263" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D263" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E263" t="s">
         <v>26</v>
@@ -7296,16 +7311,16 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B264" t="s">
         <v>6</v>
       </c>
       <c r="C264" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D264" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E264" t="s">
         <v>26</v>
@@ -7313,16 +7328,16 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B265" t="s">
         <v>6</v>
       </c>
       <c r="C265" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D265" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E265" t="s">
         <v>26</v>
@@ -7330,16 +7345,16 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B266" t="s">
         <v>6</v>
       </c>
       <c r="C266" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D266" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E266" t="s">
         <v>26</v>
@@ -7347,16 +7362,16 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B267" t="s">
         <v>6</v>
       </c>
       <c r="C267" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D267" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E267" t="s">
         <v>26</v>
@@ -7364,16 +7379,16 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B268" t="s">
         <v>6</v>
       </c>
       <c r="C268" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D268" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E268" t="s">
         <v>26</v>
@@ -7381,16 +7396,16 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B269" t="s">
         <v>76</v>
       </c>
       <c r="C269" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D269" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E269" t="s">
         <v>26</v>
@@ -7398,16 +7413,16 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
+        <v>419</v>
+      </c>
+      <c r="B270" t="s">
+        <v>6</v>
+      </c>
+      <c r="C270" t="s">
+        <v>420</v>
+      </c>
+      <c r="D270" t="s">
         <v>421</v>
-      </c>
-      <c r="B270" t="s">
-        <v>6</v>
-      </c>
-      <c r="C270" t="s">
-        <v>422</v>
-      </c>
-      <c r="D270" t="s">
-        <v>423</v>
       </c>
       <c r="E270" t="s">
         <v>26</v>
@@ -7415,16 +7430,16 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B271" t="s">
         <v>6</v>
       </c>
       <c r="C271" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D271" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E271" t="s">
         <v>26</v>
@@ -7432,16 +7447,16 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B272" t="s">
         <v>6</v>
       </c>
       <c r="C272" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D272" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E272" t="s">
         <v>26</v>
@@ -7449,16 +7464,16 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
+        <v>424</v>
+      </c>
+      <c r="B273" t="s">
+        <v>6</v>
+      </c>
+      <c r="C273" t="s">
+        <v>425</v>
+      </c>
+      <c r="D273" t="s">
         <v>426</v>
-      </c>
-      <c r="B273" t="s">
-        <v>6</v>
-      </c>
-      <c r="C273" t="s">
-        <v>427</v>
-      </c>
-      <c r="D273" t="s">
-        <v>428</v>
       </c>
       <c r="E273" t="s">
         <v>26</v>
@@ -7466,16 +7481,16 @@
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B274" t="s">
         <v>6</v>
       </c>
       <c r="C274" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D274" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E274" t="s">
         <v>26</v>
@@ -7483,16 +7498,16 @@
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B275" t="s">
         <v>6</v>
       </c>
       <c r="C275" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D275" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E275" t="s">
         <v>26</v>
@@ -7500,16 +7515,16 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B276" t="s">
         <v>6</v>
       </c>
       <c r="C276" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D276" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E276" t="s">
         <v>26</v>
@@ -7517,16 +7532,16 @@
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B277" t="s">
         <v>76</v>
       </c>
       <c r="C277" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D277" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E277" t="s">
         <v>26</v>
@@ -7534,16 +7549,16 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
+        <v>431</v>
+      </c>
+      <c r="B278" t="s">
+        <v>6</v>
+      </c>
+      <c r="C278" t="s">
+        <v>432</v>
+      </c>
+      <c r="D278" t="s">
         <v>433</v>
-      </c>
-      <c r="B278" t="s">
-        <v>6</v>
-      </c>
-      <c r="C278" t="s">
-        <v>434</v>
-      </c>
-      <c r="D278" t="s">
-        <v>435</v>
       </c>
       <c r="E278" t="s">
         <v>26</v>
@@ -7551,16 +7566,16 @@
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B279" t="s">
         <v>6</v>
       </c>
       <c r="C279" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D279" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E279" t="s">
         <v>26</v>
@@ -7568,16 +7583,16 @@
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B280" t="s">
         <v>6</v>
       </c>
       <c r="C280" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D280" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E280" t="s">
         <v>26</v>
@@ -7585,16 +7600,16 @@
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B281" t="s">
         <v>76</v>
       </c>
       <c r="C281" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D281" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E281" t="s">
         <v>26</v>
@@ -7602,16 +7617,16 @@
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
+        <v>437</v>
+      </c>
+      <c r="B282" t="s">
+        <v>6</v>
+      </c>
+      <c r="C282" t="s">
+        <v>438</v>
+      </c>
+      <c r="D282" t="s">
         <v>439</v>
-      </c>
-      <c r="B282" t="s">
-        <v>6</v>
-      </c>
-      <c r="C282" t="s">
-        <v>440</v>
-      </c>
-      <c r="D282" t="s">
-        <v>441</v>
       </c>
       <c r="E282" t="s">
         <v>26</v>
@@ -7619,16 +7634,16 @@
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B283" t="s">
         <v>6</v>
       </c>
       <c r="C283" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D283" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E283" t="s">
         <v>26</v>
@@ -7636,16 +7651,16 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
+        <v>442</v>
+      </c>
+      <c r="B284" t="s">
+        <v>6</v>
+      </c>
+      <c r="C284" t="s">
+        <v>443</v>
+      </c>
+      <c r="D284" t="s">
         <v>444</v>
-      </c>
-      <c r="B284" t="s">
-        <v>6</v>
-      </c>
-      <c r="C284" t="s">
-        <v>445</v>
-      </c>
-      <c r="D284" t="s">
-        <v>446</v>
       </c>
       <c r="E284" t="s">
         <v>26</v>
@@ -7653,16 +7668,16 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B285" t="s">
         <v>76</v>
       </c>
       <c r="C285" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D285" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E285" t="s">
         <v>26</v>
@@ -7670,16 +7685,16 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B286" t="s">
         <v>76</v>
       </c>
       <c r="C286" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D286" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E286" t="s">
         <v>26</v>
@@ -7687,16 +7702,16 @@
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
+        <v>447</v>
+      </c>
+      <c r="B287" t="s">
+        <v>6</v>
+      </c>
+      <c r="C287" t="s">
+        <v>448</v>
+      </c>
+      <c r="D287" t="s">
         <v>449</v>
-      </c>
-      <c r="B287" t="s">
-        <v>6</v>
-      </c>
-      <c r="C287" t="s">
-        <v>450</v>
-      </c>
-      <c r="D287" t="s">
-        <v>451</v>
       </c>
       <c r="E287" t="s">
         <v>26</v>
@@ -7704,16 +7719,16 @@
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B288" t="s">
         <v>6</v>
       </c>
       <c r="C288" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D288" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E288" t="s">
         <v>26</v>
@@ -7721,16 +7736,16 @@
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B289" t="s">
         <v>6</v>
       </c>
       <c r="C289" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D289" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E289" t="s">
         <v>26</v>
@@ -7738,16 +7753,16 @@
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B290" t="s">
         <v>76</v>
       </c>
       <c r="C290" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D290" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E290" t="s">
         <v>26</v>
@@ -7755,16 +7770,16 @@
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
+        <v>454</v>
+      </c>
+      <c r="B291" t="s">
+        <v>6</v>
+      </c>
+      <c r="C291" t="s">
+        <v>455</v>
+      </c>
+      <c r="D291" t="s">
         <v>456</v>
-      </c>
-      <c r="B291" t="s">
-        <v>6</v>
-      </c>
-      <c r="C291" t="s">
-        <v>457</v>
-      </c>
-      <c r="D291" t="s">
-        <v>458</v>
       </c>
       <c r="E291" t="s">
         <v>26</v>
@@ -7772,16 +7787,16 @@
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B292" t="s">
         <v>6</v>
       </c>
       <c r="C292" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D292" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E292" t="s">
         <v>26</v>
@@ -7789,16 +7804,16 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B293" t="s">
         <v>76</v>
       </c>
       <c r="C293" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D293" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E293" t="s">
         <v>26</v>
@@ -7806,16 +7821,16 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
+        <v>457</v>
+      </c>
+      <c r="B294" t="s">
+        <v>6</v>
+      </c>
+      <c r="C294" t="s">
+        <v>458</v>
+      </c>
+      <c r="D294" t="s">
         <v>459</v>
-      </c>
-      <c r="B294" t="s">
-        <v>6</v>
-      </c>
-      <c r="C294" t="s">
-        <v>460</v>
-      </c>
-      <c r="D294" t="s">
-        <v>461</v>
       </c>
       <c r="E294" t="s">
         <v>26</v>
@@ -7823,16 +7838,16 @@
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B295" t="s">
         <v>6</v>
       </c>
       <c r="C295" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D295" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E295" t="s">
         <v>26</v>
@@ -7840,16 +7855,16 @@
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B296" t="s">
         <v>76</v>
       </c>
       <c r="C296" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D296" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E296" t="s">
         <v>26</v>
@@ -7857,16 +7872,16 @@
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
+        <v>461</v>
+      </c>
+      <c r="B297" t="s">
+        <v>6</v>
+      </c>
+      <c r="C297" t="s">
+        <v>462</v>
+      </c>
+      <c r="D297" t="s">
         <v>463</v>
-      </c>
-      <c r="B297" t="s">
-        <v>6</v>
-      </c>
-      <c r="C297" t="s">
-        <v>464</v>
-      </c>
-      <c r="D297" t="s">
-        <v>465</v>
       </c>
       <c r="E297" t="s">
         <v>26</v>
@@ -7874,16 +7889,16 @@
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B298" t="s">
         <v>76</v>
       </c>
       <c r="C298" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D298" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E298" t="s">
         <v>26</v>
@@ -7891,16 +7906,16 @@
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
+        <v>467</v>
+      </c>
+      <c r="B299" t="s">
+        <v>6</v>
+      </c>
+      <c r="C299" t="s">
+        <v>468</v>
+      </c>
+      <c r="D299" t="s">
         <v>469</v>
-      </c>
-      <c r="B299" t="s">
-        <v>6</v>
-      </c>
-      <c r="C299" t="s">
-        <v>470</v>
-      </c>
-      <c r="D299" t="s">
-        <v>471</v>
       </c>
       <c r="E299" t="s">
         <v>26</v>
@@ -7908,16 +7923,16 @@
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B300" t="s">
         <v>76</v>
       </c>
       <c r="C300" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D300" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E300" t="s">
         <v>26</v>
@@ -7925,16 +7940,16 @@
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B301" t="s">
         <v>6</v>
       </c>
       <c r="C301" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D301" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E301" t="s">
         <v>26</v>
@@ -7942,16 +7957,16 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B302" t="s">
         <v>6</v>
       </c>
       <c r="C302" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D302" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="E302" t="s">
         <v>26</v>
@@ -7959,16 +7974,16 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
+        <v>474</v>
+      </c>
+      <c r="B303" t="s">
+        <v>6</v>
+      </c>
+      <c r="C303" t="s">
+        <v>475</v>
+      </c>
+      <c r="D303" t="s">
         <v>476</v>
-      </c>
-      <c r="B303" t="s">
-        <v>6</v>
-      </c>
-      <c r="C303" t="s">
-        <v>477</v>
-      </c>
-      <c r="D303" t="s">
-        <v>478</v>
       </c>
       <c r="E303" t="s">
         <v>26</v>
@@ -7976,7 +7991,7 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B304" t="s">
         <v>6</v>
@@ -7993,16 +8008,16 @@
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B305" t="s">
         <v>6</v>
       </c>
       <c r="C305" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D305" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E305" t="s">
         <v>26</v>
@@ -8010,16 +8025,16 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B306" t="s">
         <v>6</v>
       </c>
       <c r="C306" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D306" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E306" t="s">
         <v>26</v>
@@ -8027,67 +8042,67 @@
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
+        <v>491</v>
+      </c>
+      <c r="B307" t="s">
+        <v>6</v>
+      </c>
+      <c r="C307" t="s">
+        <v>492</v>
+      </c>
+      <c r="D307" t="s">
         <v>493</v>
       </c>
-      <c r="B307" t="s">
-        <v>6</v>
-      </c>
-      <c r="C307" t="s">
-        <v>494</v>
-      </c>
-      <c r="D307" t="s">
-        <v>495</v>
-      </c>
       <c r="E307" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B308" t="s">
         <v>6</v>
       </c>
       <c r="C308" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D308" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E308" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B309" t="s">
         <v>6</v>
       </c>
       <c r="C309" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D309" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E309" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B310" t="s">
         <v>6</v>
       </c>
       <c r="C310" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D310" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E310" t="s">
         <v>26</v>
@@ -8095,16 +8110,16 @@
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B311" t="s">
         <v>6</v>
       </c>
       <c r="C311" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D311" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E311" t="s">
         <v>26</v>
@@ -8112,16 +8127,16 @@
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B312" t="s">
         <v>6</v>
       </c>
       <c r="C312" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D312" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E312" t="s">
         <v>26</v>
@@ -8129,16 +8144,16 @@
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B313" t="s">
         <v>6</v>
       </c>
       <c r="C313" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D313" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E313" t="s">
         <v>9</v>
@@ -8146,16 +8161,16 @@
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B314" t="s">
         <v>6</v>
       </c>
       <c r="C314" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D314" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E314" t="s">
         <v>26</v>
@@ -8163,7 +8178,7 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B315" t="s">
         <v>6</v>
@@ -8180,16 +8195,16 @@
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B316" t="s">
         <v>6</v>
       </c>
       <c r="C316" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="D316" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E316" t="s">
         <v>26</v>
@@ -8197,16 +8212,16 @@
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B317" t="s">
         <v>6</v>
       </c>
       <c r="C317" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D317" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E317" t="s">
         <v>26</v>
@@ -8214,16 +8229,16 @@
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B318" t="s">
         <v>6</v>
       </c>
       <c r="C318" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D318" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E318" t="s">
         <v>26</v>
@@ -8231,16 +8246,16 @@
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B319" t="s">
         <v>6</v>
       </c>
       <c r="C319" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D319" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E319" t="s">
         <v>26</v>
@@ -8248,16 +8263,16 @@
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B320" t="s">
         <v>6</v>
       </c>
       <c r="C320" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D320" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E320" t="s">
         <v>26</v>
@@ -8265,7 +8280,7 @@
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B321" t="s">
         <v>6</v>
@@ -8282,16 +8297,16 @@
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B322" t="s">
         <v>6</v>
       </c>
       <c r="C322" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D322" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E322" t="s">
         <v>26</v>
@@ -8299,7 +8314,7 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B323" t="s">
         <v>6</v>
@@ -8316,13 +8331,13 @@
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B324" t="s">
         <v>6</v>
       </c>
       <c r="C324" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D324" t="s">
         <v>61</v>
@@ -8333,16 +8348,16 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B325" t="s">
         <v>6</v>
       </c>
       <c r="C325" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D325" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E325" t="s">
         <v>26</v>
@@ -8350,16 +8365,16 @@
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B326" t="s">
         <v>6</v>
       </c>
       <c r="C326" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D326" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E326" t="s">
         <v>26</v>
@@ -8367,16 +8382,16 @@
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B327" t="s">
         <v>6</v>
       </c>
       <c r="C327" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D327" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E327" t="s">
         <v>26</v>
@@ -8384,16 +8399,16 @@
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B328" t="s">
         <v>6</v>
       </c>
       <c r="C328" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D328" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E328" t="s">
         <v>26</v>
@@ -8401,16 +8416,16 @@
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B329" t="s">
         <v>6</v>
       </c>
       <c r="C329" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D329" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E329" t="s">
         <v>26</v>
@@ -8418,16 +8433,16 @@
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B330" t="s">
         <v>6</v>
       </c>
       <c r="C330" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D330" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E330" t="s">
         <v>26</v>
@@ -8435,16 +8450,16 @@
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B331" t="s">
         <v>6</v>
       </c>
       <c r="C331" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D331" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E331" t="s">
         <v>26</v>
@@ -8452,16 +8467,16 @@
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B332" t="s">
         <v>6</v>
       </c>
       <c r="C332" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D332" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E332" t="s">
         <v>26</v>
@@ -8469,16 +8484,16 @@
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B333" t="s">
         <v>6</v>
       </c>
       <c r="C333" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D333" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E333" t="s">
         <v>26</v>
@@ -8486,16 +8501,16 @@
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B334" t="s">
         <v>6</v>
       </c>
       <c r="C334" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D334" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E334" t="s">
         <v>26</v>
@@ -8503,16 +8518,16 @@
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B335" t="s">
         <v>6</v>
       </c>
       <c r="C335" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D335" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E335" t="s">
         <v>26</v>
@@ -8520,16 +8535,16 @@
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B336" t="s">
         <v>6</v>
       </c>
       <c r="C336" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D336" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E336" t="s">
         <v>26</v>
@@ -8537,16 +8552,16 @@
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B337" t="s">
         <v>6</v>
       </c>
       <c r="C337" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D337" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E337" t="s">
         <v>26</v>
@@ -8554,16 +8569,16 @@
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B338" t="s">
         <v>6</v>
       </c>
       <c r="C338" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D338" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E338" t="s">
         <v>26</v>
@@ -8571,16 +8586,16 @@
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B339" t="s">
         <v>6</v>
       </c>
       <c r="C339" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D339" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E339" t="s">
         <v>26</v>
@@ -8588,16 +8603,16 @@
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B340" t="s">
         <v>6</v>
       </c>
       <c r="C340" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D340" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E340" t="s">
         <v>26</v>
@@ -8605,16 +8620,16 @@
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B341" t="s">
         <v>6</v>
       </c>
       <c r="C341" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D341" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E341" t="s">
         <v>26</v>
@@ -8622,16 +8637,16 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B342" t="s">
         <v>6</v>
       </c>
       <c r="C342" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D342" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E342" t="s">
         <v>26</v>
@@ -8639,16 +8654,16 @@
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B343" t="s">
         <v>6</v>
       </c>
       <c r="C343" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D343" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E343" t="s">
         <v>26</v>
@@ -8656,7 +8671,7 @@
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B344" t="s">
         <v>76</v>
@@ -8673,16 +8688,16 @@
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B345" t="s">
         <v>6</v>
       </c>
       <c r="C345" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D345" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E345" t="s">
         <v>9</v>
@@ -8690,16 +8705,16 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B346" t="s">
         <v>6</v>
       </c>
       <c r="C346" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D346" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E346" t="s">
         <v>9</v>
@@ -8707,16 +8722,16 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B347" t="s">
         <v>76</v>
       </c>
       <c r="C347" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D347" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E347" t="s">
         <v>9</v>
@@ -8724,16 +8739,16 @@
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B348" t="s">
         <v>76</v>
       </c>
       <c r="C348" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D348" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E348" t="s">
         <v>9</v>
@@ -8741,16 +8756,16 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B349" t="s">
         <v>6</v>
       </c>
       <c r="C349" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D349" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E349" t="s">
         <v>9</v>
@@ -8758,16 +8773,16 @@
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B350" t="s">
         <v>6</v>
       </c>
       <c r="C350" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D350" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E350" t="s">
         <v>26</v>
@@ -8775,7 +8790,7 @@
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A351" s="2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B351" t="s">
         <v>6</v>

</xml_diff>